<commit_message>
Đã thiết kế lại DB mới theo yêu cầu trong file Project HaiPM
</commit_message>
<xml_diff>
--- a/ projectquanlybongdavodichquocgia/Document/Specify/SPECIFY PROJECT.xlsx
+++ b/ projectquanlybongdavodichquocgia/Document/Specify/SPECIFY PROJECT.xlsx
@@ -890,7 +890,7 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="114">
+  <cellXfs count="116">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="13" xfId="19" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
@@ -1011,6 +1011,12 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="15" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="15" fillId="5" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="0" xfId="26" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="32" xfId="26" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="31" xfId="26" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -1053,21 +1059,6 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="26" xfId="26" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="0" xfId="26" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="32" xfId="26" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="2" borderId="11" xfId="19" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="2" borderId="2" xfId="19" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="2" borderId="10" xfId="19" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="12" fillId="5" borderId="11" xfId="19" applyFont="1" applyFill="1" applyBorder="1">
       <alignment vertical="center"/>
     </xf>
@@ -1077,31 +1068,10 @@
     <xf numFmtId="0" fontId="12" fillId="5" borderId="10" xfId="19" applyFont="1" applyFill="1" applyBorder="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="2" borderId="18" xfId="19" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="12" fillId="2" borderId="11" xfId="19" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="2" borderId="5" xfId="19" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="2" borderId="19" xfId="19" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="14" fontId="12" fillId="0" borderId="11" xfId="19" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="2" xfId="19" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="13" xfId="19" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="11" xfId="19" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="5" xfId="19" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="19" xfId="19" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="12" fillId="2" borderId="2" xfId="19" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="12" fillId="2" borderId="13" xfId="19" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1123,6 +1093,60 @@
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="12" fillId="2" borderId="10" xfId="19" applyFont="1" applyFill="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="2" borderId="18" xfId="19" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="2" borderId="5" xfId="19" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="2" borderId="19" xfId="19" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="2" borderId="10" xfId="19" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="12" fillId="0" borderId="11" xfId="19" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="2" xfId="19" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="13" xfId="19" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="11" xfId="19" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="5" xfId="19" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="19" xfId="19" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="2" borderId="11" xfId="19" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="2" borderId="2" xfId="19" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="2" borderId="10" xfId="19" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="11" xfId="19" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="2" xfId="19" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="9" xfId="19" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="19" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="10" xfId="19" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="11" xfId="19" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1161,28 +1185,10 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="11" xfId="19" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="17" fillId="2" borderId="11" xfId="19" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="2" borderId="2" xfId="19" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="2" borderId="10" xfId="19" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="17" fillId="0" borderId="11" xfId="19" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+      <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="17" fillId="0" borderId="2" xfId="19" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="9" xfId="19" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="19" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="10" xfId="19" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
   </cellXfs>
@@ -2864,8 +2870,8 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="0" orientation="portrait" horizontalDpi="0" verticalDpi="0" copies="0"/>
-  <drawing r:id="rId1"/>
+  <pageSetup orientation="portrait" horizontalDpi="200" verticalDpi="200" copies="0" r:id="rId1"/>
+  <drawing r:id="rId2"/>
 </worksheet>
 </file>
 
@@ -2948,38 +2954,38 @@
       <c r="L2" s="14"/>
       <c r="M2" s="14"/>
       <c r="N2" s="14"/>
-      <c r="O2" s="70" t="s">
+      <c r="O2" s="56" t="s">
         <v>8</v>
       </c>
-      <c r="P2" s="70"/>
-      <c r="Q2" s="70"/>
-      <c r="R2" s="70"/>
-      <c r="S2" s="70"/>
-      <c r="T2" s="70"/>
-      <c r="U2" s="70"/>
-      <c r="V2" s="70"/>
-      <c r="W2" s="70"/>
-      <c r="X2" s="70"/>
-      <c r="Y2" s="70"/>
-      <c r="Z2" s="70"/>
-      <c r="AA2" s="70"/>
-      <c r="AB2" s="70"/>
-      <c r="AC2" s="70"/>
-      <c r="AD2" s="70"/>
-      <c r="AE2" s="70"/>
-      <c r="AF2" s="70"/>
-      <c r="AG2" s="70"/>
-      <c r="AH2" s="70"/>
-      <c r="AI2" s="70"/>
-      <c r="AJ2" s="70"/>
-      <c r="AK2" s="70"/>
-      <c r="AL2" s="70"/>
-      <c r="AM2" s="70"/>
-      <c r="AN2" s="70"/>
-      <c r="AO2" s="70"/>
-      <c r="AP2" s="70"/>
-      <c r="AQ2" s="70"/>
-      <c r="AR2" s="70"/>
+      <c r="P2" s="56"/>
+      <c r="Q2" s="56"/>
+      <c r="R2" s="56"/>
+      <c r="S2" s="56"/>
+      <c r="T2" s="56"/>
+      <c r="U2" s="56"/>
+      <c r="V2" s="56"/>
+      <c r="W2" s="56"/>
+      <c r="X2" s="56"/>
+      <c r="Y2" s="56"/>
+      <c r="Z2" s="56"/>
+      <c r="AA2" s="56"/>
+      <c r="AB2" s="56"/>
+      <c r="AC2" s="56"/>
+      <c r="AD2" s="56"/>
+      <c r="AE2" s="56"/>
+      <c r="AF2" s="56"/>
+      <c r="AG2" s="56"/>
+      <c r="AH2" s="56"/>
+      <c r="AI2" s="56"/>
+      <c r="AJ2" s="56"/>
+      <c r="AK2" s="56"/>
+      <c r="AL2" s="56"/>
+      <c r="AM2" s="56"/>
+      <c r="AN2" s="56"/>
+      <c r="AO2" s="56"/>
+      <c r="AP2" s="56"/>
+      <c r="AQ2" s="56"/>
+      <c r="AR2" s="56"/>
       <c r="AS2" s="14"/>
       <c r="AT2" s="14"/>
       <c r="AU2" s="14"/>
@@ -3088,228 +3094,223 @@
       <c r="AV4" s="14"/>
     </row>
     <row r="5" spans="1:48">
-      <c r="A5" s="71" t="s">
+      <c r="A5" s="57" t="s">
         <v>0</v>
       </c>
-      <c r="B5" s="56"/>
-      <c r="C5" s="56" t="s">
+      <c r="B5" s="58"/>
+      <c r="C5" s="58" t="s">
         <v>1</v>
       </c>
-      <c r="D5" s="56"/>
-      <c r="E5" s="56"/>
-      <c r="F5" s="56"/>
-      <c r="G5" s="56"/>
-      <c r="H5" s="56"/>
-      <c r="I5" s="56"/>
-      <c r="J5" s="56"/>
-      <c r="K5" s="56"/>
-      <c r="L5" s="56"/>
-      <c r="M5" s="56"/>
-      <c r="N5" s="56"/>
-      <c r="O5" s="56" t="s">
+      <c r="D5" s="58"/>
+      <c r="E5" s="58"/>
+      <c r="F5" s="58"/>
+      <c r="G5" s="58"/>
+      <c r="H5" s="58"/>
+      <c r="I5" s="58"/>
+      <c r="J5" s="58"/>
+      <c r="K5" s="58"/>
+      <c r="L5" s="58"/>
+      <c r="M5" s="58"/>
+      <c r="N5" s="58"/>
+      <c r="O5" s="58" t="s">
         <v>12</v>
       </c>
-      <c r="P5" s="56"/>
-      <c r="Q5" s="56"/>
-      <c r="R5" s="56"/>
-      <c r="S5" s="56"/>
-      <c r="T5" s="56"/>
-      <c r="U5" s="56"/>
-      <c r="V5" s="56"/>
-      <c r="W5" s="56"/>
-      <c r="X5" s="56"/>
-      <c r="Y5" s="56"/>
-      <c r="Z5" s="56"/>
-      <c r="AA5" s="56"/>
-      <c r="AB5" s="56"/>
-      <c r="AC5" s="56"/>
-      <c r="AD5" s="56"/>
-      <c r="AE5" s="56"/>
-      <c r="AF5" s="56"/>
-      <c r="AG5" s="56"/>
-      <c r="AH5" s="56"/>
-      <c r="AI5" s="56"/>
-      <c r="AJ5" s="56"/>
-      <c r="AK5" s="56"/>
-      <c r="AL5" s="56"/>
-      <c r="AM5" s="56"/>
-      <c r="AN5" s="56"/>
-      <c r="AO5" s="56"/>
-      <c r="AP5" s="56"/>
-      <c r="AQ5" s="56"/>
-      <c r="AR5" s="56"/>
-      <c r="AS5" s="56" t="s">
+      <c r="P5" s="58"/>
+      <c r="Q5" s="58"/>
+      <c r="R5" s="58"/>
+      <c r="S5" s="58"/>
+      <c r="T5" s="58"/>
+      <c r="U5" s="58"/>
+      <c r="V5" s="58"/>
+      <c r="W5" s="58"/>
+      <c r="X5" s="58"/>
+      <c r="Y5" s="58"/>
+      <c r="Z5" s="58"/>
+      <c r="AA5" s="58"/>
+      <c r="AB5" s="58"/>
+      <c r="AC5" s="58"/>
+      <c r="AD5" s="58"/>
+      <c r="AE5" s="58"/>
+      <c r="AF5" s="58"/>
+      <c r="AG5" s="58"/>
+      <c r="AH5" s="58"/>
+      <c r="AI5" s="58"/>
+      <c r="AJ5" s="58"/>
+      <c r="AK5" s="58"/>
+      <c r="AL5" s="58"/>
+      <c r="AM5" s="58"/>
+      <c r="AN5" s="58"/>
+      <c r="AO5" s="58"/>
+      <c r="AP5" s="58"/>
+      <c r="AQ5" s="58"/>
+      <c r="AR5" s="58"/>
+      <c r="AS5" s="58" t="s">
         <v>2</v>
       </c>
-      <c r="AT5" s="56"/>
-      <c r="AU5" s="56"/>
-      <c r="AV5" s="56"/>
+      <c r="AT5" s="58"/>
+      <c r="AU5" s="58"/>
+      <c r="AV5" s="58"/>
     </row>
     <row r="6" spans="1:48">
-      <c r="A6" s="64">
+      <c r="A6" s="66">
         <v>1</v>
       </c>
-      <c r="B6" s="65"/>
-      <c r="C6" s="66">
+      <c r="B6" s="67"/>
+      <c r="C6" s="68">
         <v>40997</v>
       </c>
-      <c r="D6" s="67"/>
-      <c r="E6" s="67"/>
-      <c r="F6" s="67"/>
-      <c r="G6" s="68"/>
-      <c r="H6" s="65"/>
-      <c r="I6" s="65"/>
-      <c r="J6" s="65"/>
-      <c r="K6" s="65"/>
-      <c r="L6" s="65"/>
-      <c r="M6" s="65"/>
-      <c r="N6" s="65"/>
-      <c r="O6" s="69" t="s">
+      <c r="D6" s="69"/>
+      <c r="E6" s="69"/>
+      <c r="F6" s="69"/>
+      <c r="G6" s="70"/>
+      <c r="H6" s="67"/>
+      <c r="I6" s="67"/>
+      <c r="J6" s="67"/>
+      <c r="K6" s="67"/>
+      <c r="L6" s="67"/>
+      <c r="M6" s="67"/>
+      <c r="N6" s="67"/>
+      <c r="O6" s="71" t="s">
         <v>11</v>
       </c>
-      <c r="P6" s="69"/>
-      <c r="Q6" s="69"/>
-      <c r="R6" s="69"/>
-      <c r="S6" s="69"/>
-      <c r="T6" s="69"/>
-      <c r="U6" s="69"/>
-      <c r="V6" s="69"/>
-      <c r="W6" s="69"/>
-      <c r="X6" s="69"/>
-      <c r="Y6" s="69"/>
-      <c r="Z6" s="69"/>
-      <c r="AA6" s="69"/>
-      <c r="AB6" s="69"/>
-      <c r="AC6" s="69"/>
-      <c r="AD6" s="69"/>
-      <c r="AE6" s="69"/>
-      <c r="AF6" s="69"/>
-      <c r="AG6" s="69"/>
-      <c r="AH6" s="69"/>
-      <c r="AI6" s="69"/>
-      <c r="AJ6" s="69"/>
-      <c r="AK6" s="69"/>
-      <c r="AL6" s="69"/>
-      <c r="AM6" s="69"/>
-      <c r="AN6" s="69"/>
-      <c r="AO6" s="69"/>
-      <c r="AP6" s="69"/>
-      <c r="AQ6" s="69"/>
-      <c r="AR6" s="69"/>
-      <c r="AS6" s="63" t="s">
+      <c r="P6" s="71"/>
+      <c r="Q6" s="71"/>
+      <c r="R6" s="71"/>
+      <c r="S6" s="71"/>
+      <c r="T6" s="71"/>
+      <c r="U6" s="71"/>
+      <c r="V6" s="71"/>
+      <c r="W6" s="71"/>
+      <c r="X6" s="71"/>
+      <c r="Y6" s="71"/>
+      <c r="Z6" s="71"/>
+      <c r="AA6" s="71"/>
+      <c r="AB6" s="71"/>
+      <c r="AC6" s="71"/>
+      <c r="AD6" s="71"/>
+      <c r="AE6" s="71"/>
+      <c r="AF6" s="71"/>
+      <c r="AG6" s="71"/>
+      <c r="AH6" s="71"/>
+      <c r="AI6" s="71"/>
+      <c r="AJ6" s="71"/>
+      <c r="AK6" s="71"/>
+      <c r="AL6" s="71"/>
+      <c r="AM6" s="71"/>
+      <c r="AN6" s="71"/>
+      <c r="AO6" s="71"/>
+      <c r="AP6" s="71"/>
+      <c r="AQ6" s="71"/>
+      <c r="AR6" s="71"/>
+      <c r="AS6" s="65" t="s">
         <v>3</v>
       </c>
-      <c r="AT6" s="63"/>
-      <c r="AU6" s="63"/>
-      <c r="AV6" s="63"/>
+      <c r="AT6" s="65"/>
+      <c r="AU6" s="65"/>
+      <c r="AV6" s="65"/>
     </row>
     <row r="7" spans="1:48">
-      <c r="A7" s="58"/>
-      <c r="B7" s="57"/>
-      <c r="C7" s="59"/>
-      <c r="D7" s="60"/>
-      <c r="E7" s="60"/>
-      <c r="F7" s="60"/>
-      <c r="G7" s="61"/>
-      <c r="H7" s="57"/>
-      <c r="I7" s="57"/>
-      <c r="J7" s="57"/>
-      <c r="K7" s="57"/>
-      <c r="L7" s="57"/>
-      <c r="M7" s="57"/>
-      <c r="N7" s="57"/>
-      <c r="O7" s="62"/>
-      <c r="P7" s="62"/>
-      <c r="Q7" s="62"/>
-      <c r="R7" s="62"/>
-      <c r="S7" s="62"/>
-      <c r="T7" s="62"/>
-      <c r="U7" s="62"/>
-      <c r="V7" s="62"/>
-      <c r="W7" s="62"/>
-      <c r="X7" s="62"/>
-      <c r="Y7" s="62"/>
-      <c r="Z7" s="62"/>
-      <c r="AA7" s="62"/>
-      <c r="AB7" s="62"/>
-      <c r="AC7" s="62"/>
-      <c r="AD7" s="62"/>
-      <c r="AE7" s="62"/>
-      <c r="AF7" s="62"/>
-      <c r="AG7" s="62"/>
-      <c r="AH7" s="62"/>
-      <c r="AI7" s="62"/>
-      <c r="AJ7" s="62"/>
-      <c r="AK7" s="62"/>
-      <c r="AL7" s="62"/>
-      <c r="AM7" s="62"/>
-      <c r="AN7" s="62"/>
-      <c r="AO7" s="62"/>
-      <c r="AP7" s="62"/>
-      <c r="AQ7" s="62"/>
-      <c r="AR7" s="62"/>
-      <c r="AS7" s="57"/>
-      <c r="AT7" s="57"/>
-      <c r="AU7" s="57"/>
-      <c r="AV7" s="57"/>
+      <c r="A7" s="60"/>
+      <c r="B7" s="59"/>
+      <c r="C7" s="61"/>
+      <c r="D7" s="62"/>
+      <c r="E7" s="62"/>
+      <c r="F7" s="62"/>
+      <c r="G7" s="63"/>
+      <c r="H7" s="59"/>
+      <c r="I7" s="59"/>
+      <c r="J7" s="59"/>
+      <c r="K7" s="59"/>
+      <c r="L7" s="59"/>
+      <c r="M7" s="59"/>
+      <c r="N7" s="59"/>
+      <c r="O7" s="64"/>
+      <c r="P7" s="64"/>
+      <c r="Q7" s="64"/>
+      <c r="R7" s="64"/>
+      <c r="S7" s="64"/>
+      <c r="T7" s="64"/>
+      <c r="U7" s="64"/>
+      <c r="V7" s="64"/>
+      <c r="W7" s="64"/>
+      <c r="X7" s="64"/>
+      <c r="Y7" s="64"/>
+      <c r="Z7" s="64"/>
+      <c r="AA7" s="64"/>
+      <c r="AB7" s="64"/>
+      <c r="AC7" s="64"/>
+      <c r="AD7" s="64"/>
+      <c r="AE7" s="64"/>
+      <c r="AF7" s="64"/>
+      <c r="AG7" s="64"/>
+      <c r="AH7" s="64"/>
+      <c r="AI7" s="64"/>
+      <c r="AJ7" s="64"/>
+      <c r="AK7" s="64"/>
+      <c r="AL7" s="64"/>
+      <c r="AM7" s="64"/>
+      <c r="AN7" s="64"/>
+      <c r="AO7" s="64"/>
+      <c r="AP7" s="64"/>
+      <c r="AQ7" s="64"/>
+      <c r="AR7" s="64"/>
+      <c r="AS7" s="59"/>
+      <c r="AT7" s="59"/>
+      <c r="AU7" s="59"/>
+      <c r="AV7" s="59"/>
     </row>
     <row r="8" spans="1:48">
-      <c r="A8" s="58"/>
-      <c r="B8" s="57"/>
-      <c r="C8" s="59"/>
-      <c r="D8" s="60"/>
-      <c r="E8" s="60"/>
-      <c r="F8" s="60"/>
-      <c r="G8" s="61"/>
-      <c r="H8" s="57"/>
-      <c r="I8" s="57"/>
-      <c r="J8" s="57"/>
-      <c r="K8" s="57"/>
-      <c r="L8" s="57"/>
-      <c r="M8" s="57"/>
-      <c r="N8" s="57"/>
-      <c r="O8" s="62"/>
-      <c r="P8" s="62"/>
-      <c r="Q8" s="62"/>
-      <c r="R8" s="62"/>
-      <c r="S8" s="62"/>
-      <c r="T8" s="62"/>
-      <c r="U8" s="62"/>
-      <c r="V8" s="62"/>
-      <c r="W8" s="62"/>
-      <c r="X8" s="62"/>
-      <c r="Y8" s="62"/>
-      <c r="Z8" s="62"/>
-      <c r="AA8" s="62"/>
-      <c r="AB8" s="62"/>
-      <c r="AC8" s="62"/>
-      <c r="AD8" s="62"/>
-      <c r="AE8" s="62"/>
-      <c r="AF8" s="62"/>
-      <c r="AG8" s="62"/>
-      <c r="AH8" s="62"/>
-      <c r="AI8" s="62"/>
-      <c r="AJ8" s="62"/>
-      <c r="AK8" s="62"/>
-      <c r="AL8" s="62"/>
-      <c r="AM8" s="62"/>
-      <c r="AN8" s="62"/>
-      <c r="AO8" s="62"/>
-      <c r="AP8" s="62"/>
-      <c r="AQ8" s="62"/>
-      <c r="AR8" s="62"/>
-      <c r="AS8" s="57"/>
-      <c r="AT8" s="57"/>
-      <c r="AU8" s="57"/>
-      <c r="AV8" s="57"/>
+      <c r="A8" s="60"/>
+      <c r="B8" s="59"/>
+      <c r="C8" s="61"/>
+      <c r="D8" s="62"/>
+      <c r="E8" s="62"/>
+      <c r="F8" s="62"/>
+      <c r="G8" s="63"/>
+      <c r="H8" s="59"/>
+      <c r="I8" s="59"/>
+      <c r="J8" s="59"/>
+      <c r="K8" s="59"/>
+      <c r="L8" s="59"/>
+      <c r="M8" s="59"/>
+      <c r="N8" s="59"/>
+      <c r="O8" s="64"/>
+      <c r="P8" s="64"/>
+      <c r="Q8" s="64"/>
+      <c r="R8" s="64"/>
+      <c r="S8" s="64"/>
+      <c r="T8" s="64"/>
+      <c r="U8" s="64"/>
+      <c r="V8" s="64"/>
+      <c r="W8" s="64"/>
+      <c r="X8" s="64"/>
+      <c r="Y8" s="64"/>
+      <c r="Z8" s="64"/>
+      <c r="AA8" s="64"/>
+      <c r="AB8" s="64"/>
+      <c r="AC8" s="64"/>
+      <c r="AD8" s="64"/>
+      <c r="AE8" s="64"/>
+      <c r="AF8" s="64"/>
+      <c r="AG8" s="64"/>
+      <c r="AH8" s="64"/>
+      <c r="AI8" s="64"/>
+      <c r="AJ8" s="64"/>
+      <c r="AK8" s="64"/>
+      <c r="AL8" s="64"/>
+      <c r="AM8" s="64"/>
+      <c r="AN8" s="64"/>
+      <c r="AO8" s="64"/>
+      <c r="AP8" s="64"/>
+      <c r="AQ8" s="64"/>
+      <c r="AR8" s="64"/>
+      <c r="AS8" s="59"/>
+      <c r="AT8" s="59"/>
+      <c r="AU8" s="59"/>
+      <c r="AV8" s="59"/>
     </row>
   </sheetData>
   <mergeCells count="21">
-    <mergeCell ref="O2:AR2"/>
-    <mergeCell ref="A5:B5"/>
-    <mergeCell ref="C5:G5"/>
-    <mergeCell ref="H5:N5"/>
-    <mergeCell ref="O5:AR5"/>
     <mergeCell ref="AS5:AV5"/>
     <mergeCell ref="AS8:AV8"/>
     <mergeCell ref="A8:B8"/>
@@ -3326,9 +3327,14 @@
     <mergeCell ref="C7:G7"/>
     <mergeCell ref="H7:N7"/>
     <mergeCell ref="O7:AR7"/>
+    <mergeCell ref="O2:AR2"/>
+    <mergeCell ref="A5:B5"/>
+    <mergeCell ref="C5:G5"/>
+    <mergeCell ref="H5:N5"/>
+    <mergeCell ref="O5:AR5"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="0" orientation="portrait" horizontalDpi="0" verticalDpi="0" copies="0"/>
+  <pageSetup orientation="portrait" horizontalDpi="200" verticalDpi="200" copies="0" r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -3349,69 +3355,69 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:61">
-      <c r="A1" s="72" t="s">
+      <c r="A1" s="75" t="s">
         <v>4</v>
       </c>
-      <c r="B1" s="73"/>
-      <c r="C1" s="73"/>
-      <c r="D1" s="73"/>
-      <c r="E1" s="73"/>
-      <c r="F1" s="73"/>
-      <c r="G1" s="73"/>
-      <c r="H1" s="73"/>
-      <c r="I1" s="73"/>
-      <c r="J1" s="73"/>
-      <c r="K1" s="73"/>
-      <c r="L1" s="73"/>
-      <c r="M1" s="73"/>
-      <c r="N1" s="73"/>
-      <c r="O1" s="74"/>
-      <c r="P1" s="85" t="str">
+      <c r="B1" s="76"/>
+      <c r="C1" s="76"/>
+      <c r="D1" s="76"/>
+      <c r="E1" s="76"/>
+      <c r="F1" s="76"/>
+      <c r="G1" s="76"/>
+      <c r="H1" s="76"/>
+      <c r="I1" s="76"/>
+      <c r="J1" s="76"/>
+      <c r="K1" s="76"/>
+      <c r="L1" s="76"/>
+      <c r="M1" s="76"/>
+      <c r="N1" s="76"/>
+      <c r="O1" s="87"/>
+      <c r="P1" s="92" t="str">
         <f>'History(Lich Su)'!A4</f>
         <v>Quản Lý Giải Vô Địch Bóng Đá Quốc Gia</v>
       </c>
-      <c r="Q1" s="85"/>
-      <c r="R1" s="85"/>
-      <c r="S1" s="85"/>
-      <c r="T1" s="85"/>
-      <c r="U1" s="85"/>
-      <c r="V1" s="85"/>
-      <c r="W1" s="85"/>
-      <c r="X1" s="85"/>
-      <c r="Y1" s="85"/>
-      <c r="Z1" s="85"/>
-      <c r="AA1" s="85"/>
-      <c r="AB1" s="85"/>
-      <c r="AC1" s="85"/>
-      <c r="AD1" s="85"/>
-      <c r="AE1" s="85"/>
-      <c r="AF1" s="85"/>
-      <c r="AG1" s="85"/>
-      <c r="AH1" s="86"/>
-      <c r="AI1" s="78" t="s">
+      <c r="Q1" s="92"/>
+      <c r="R1" s="92"/>
+      <c r="S1" s="92"/>
+      <c r="T1" s="92"/>
+      <c r="U1" s="92"/>
+      <c r="V1" s="92"/>
+      <c r="W1" s="92"/>
+      <c r="X1" s="92"/>
+      <c r="Y1" s="92"/>
+      <c r="Z1" s="92"/>
+      <c r="AA1" s="92"/>
+      <c r="AB1" s="92"/>
+      <c r="AC1" s="92"/>
+      <c r="AD1" s="92"/>
+      <c r="AE1" s="92"/>
+      <c r="AF1" s="92"/>
+      <c r="AG1" s="92"/>
+      <c r="AH1" s="93"/>
+      <c r="AI1" s="84" t="s">
         <v>1</v>
       </c>
-      <c r="AJ1" s="79"/>
-      <c r="AK1" s="79"/>
-      <c r="AL1" s="79"/>
-      <c r="AM1" s="80"/>
-      <c r="AN1" s="81">
+      <c r="AJ1" s="85"/>
+      <c r="AK1" s="85"/>
+      <c r="AL1" s="85"/>
+      <c r="AM1" s="86"/>
+      <c r="AN1" s="88">
         <f>'History(Lich Su)'!C6</f>
         <v>40997</v>
       </c>
-      <c r="AO1" s="82"/>
-      <c r="AP1" s="82"/>
-      <c r="AQ1" s="82"/>
-      <c r="AR1" s="82"/>
-      <c r="AS1" s="82"/>
-      <c r="AT1" s="82"/>
-      <c r="AU1" s="82"/>
-      <c r="AV1" s="82"/>
-      <c r="AW1" s="82"/>
-      <c r="AX1" s="82"/>
-      <c r="AY1" s="82"/>
-      <c r="AZ1" s="82"/>
-      <c r="BA1" s="83"/>
+      <c r="AO1" s="89"/>
+      <c r="AP1" s="89"/>
+      <c r="AQ1" s="89"/>
+      <c r="AR1" s="89"/>
+      <c r="AS1" s="89"/>
+      <c r="AT1" s="89"/>
+      <c r="AU1" s="89"/>
+      <c r="AV1" s="89"/>
+      <c r="AW1" s="89"/>
+      <c r="AX1" s="89"/>
+      <c r="AY1" s="89"/>
+      <c r="AZ1" s="89"/>
+      <c r="BA1" s="90"/>
     </row>
     <row r="2" spans="1:61">
       <c r="A2" s="22"/>
@@ -3448,41 +3454,41 @@
       <c r="AF2" s="23"/>
       <c r="AG2" s="23"/>
       <c r="AH2" s="24"/>
-      <c r="AI2" s="72" t="s">
+      <c r="AI2" s="75" t="s">
         <v>2</v>
       </c>
-      <c r="AJ2" s="73"/>
-      <c r="AK2" s="73"/>
-      <c r="AL2" s="73"/>
-      <c r="AM2" s="74"/>
-      <c r="AN2" s="84" t="str">
+      <c r="AJ2" s="76"/>
+      <c r="AK2" s="76"/>
+      <c r="AL2" s="76"/>
+      <c r="AM2" s="87"/>
+      <c r="AN2" s="91" t="str">
         <f>'History(Lich Su)'!AS6</f>
         <v>HaiPM</v>
       </c>
-      <c r="AO2" s="82"/>
-      <c r="AP2" s="82"/>
-      <c r="AQ2" s="82"/>
-      <c r="AR2" s="82"/>
-      <c r="AS2" s="82"/>
-      <c r="AT2" s="82"/>
-      <c r="AU2" s="82"/>
-      <c r="AV2" s="82"/>
-      <c r="AW2" s="82"/>
-      <c r="AX2" s="82"/>
-      <c r="AY2" s="82"/>
-      <c r="AZ2" s="82"/>
-      <c r="BA2" s="83"/>
+      <c r="AO2" s="89"/>
+      <c r="AP2" s="89"/>
+      <c r="AQ2" s="89"/>
+      <c r="AR2" s="89"/>
+      <c r="AS2" s="89"/>
+      <c r="AT2" s="89"/>
+      <c r="AU2" s="89"/>
+      <c r="AV2" s="89"/>
+      <c r="AW2" s="89"/>
+      <c r="AX2" s="89"/>
+      <c r="AY2" s="89"/>
+      <c r="AZ2" s="89"/>
+      <c r="BA2" s="90"/>
     </row>
     <row r="3" spans="1:61">
-      <c r="A3" s="88" t="s">
+      <c r="A3" s="78" t="s">
         <v>5</v>
       </c>
-      <c r="B3" s="73"/>
-      <c r="C3" s="73"/>
-      <c r="D3" s="73"/>
-      <c r="E3" s="73"/>
-      <c r="F3" s="73"/>
-      <c r="G3" s="87"/>
+      <c r="B3" s="76"/>
+      <c r="C3" s="76"/>
+      <c r="D3" s="76"/>
+      <c r="E3" s="76"/>
+      <c r="F3" s="76"/>
+      <c r="G3" s="77"/>
       <c r="H3" s="23" t="str">
         <f>'History(Lich Su)'!A4</f>
         <v>Quản Lý Giải Vô Địch Bóng Đá Quốc Gia</v>
@@ -3537,64 +3543,64 @@
       <c r="A4" s="26" t="s">
         <v>0</v>
       </c>
-      <c r="B4" s="89" t="s">
+      <c r="B4" s="79" t="s">
         <v>14</v>
       </c>
-      <c r="C4" s="90"/>
-      <c r="D4" s="90"/>
-      <c r="E4" s="90"/>
-      <c r="F4" s="90"/>
-      <c r="G4" s="90"/>
-      <c r="H4" s="90"/>
-      <c r="I4" s="90"/>
-      <c r="J4" s="90"/>
-      <c r="K4" s="90"/>
-      <c r="L4" s="90"/>
-      <c r="M4" s="91" t="s">
+      <c r="C4" s="80"/>
+      <c r="D4" s="80"/>
+      <c r="E4" s="80"/>
+      <c r="F4" s="80"/>
+      <c r="G4" s="80"/>
+      <c r="H4" s="80"/>
+      <c r="I4" s="80"/>
+      <c r="J4" s="80"/>
+      <c r="K4" s="80"/>
+      <c r="L4" s="80"/>
+      <c r="M4" s="81" t="s">
         <v>16</v>
       </c>
-      <c r="N4" s="92"/>
-      <c r="O4" s="92"/>
-      <c r="P4" s="92"/>
-      <c r="Q4" s="92"/>
-      <c r="R4" s="93"/>
-      <c r="S4" s="72" t="s">
+      <c r="N4" s="82"/>
+      <c r="O4" s="82"/>
+      <c r="P4" s="82"/>
+      <c r="Q4" s="82"/>
+      <c r="R4" s="83"/>
+      <c r="S4" s="75" t="s">
         <v>15</v>
       </c>
-      <c r="T4" s="73"/>
-      <c r="U4" s="73"/>
-      <c r="V4" s="73"/>
-      <c r="W4" s="73"/>
-      <c r="X4" s="73"/>
-      <c r="Y4" s="73"/>
-      <c r="Z4" s="73"/>
-      <c r="AA4" s="73"/>
-      <c r="AB4" s="73"/>
-      <c r="AC4" s="73"/>
-      <c r="AD4" s="73"/>
-      <c r="AE4" s="73"/>
-      <c r="AF4" s="73"/>
-      <c r="AG4" s="73"/>
-      <c r="AH4" s="73"/>
-      <c r="AI4" s="73"/>
-      <c r="AJ4" s="73"/>
-      <c r="AK4" s="73"/>
-      <c r="AL4" s="73"/>
-      <c r="AM4" s="73"/>
-      <c r="AN4" s="73"/>
-      <c r="AO4" s="73"/>
-      <c r="AP4" s="73"/>
-      <c r="AQ4" s="73"/>
-      <c r="AR4" s="73"/>
-      <c r="AS4" s="73"/>
-      <c r="AT4" s="73"/>
-      <c r="AU4" s="73"/>
-      <c r="AV4" s="73"/>
-      <c r="AW4" s="73"/>
-      <c r="AX4" s="73"/>
-      <c r="AY4" s="73"/>
-      <c r="AZ4" s="73"/>
-      <c r="BA4" s="87"/>
+      <c r="T4" s="76"/>
+      <c r="U4" s="76"/>
+      <c r="V4" s="76"/>
+      <c r="W4" s="76"/>
+      <c r="X4" s="76"/>
+      <c r="Y4" s="76"/>
+      <c r="Z4" s="76"/>
+      <c r="AA4" s="76"/>
+      <c r="AB4" s="76"/>
+      <c r="AC4" s="76"/>
+      <c r="AD4" s="76"/>
+      <c r="AE4" s="76"/>
+      <c r="AF4" s="76"/>
+      <c r="AG4" s="76"/>
+      <c r="AH4" s="76"/>
+      <c r="AI4" s="76"/>
+      <c r="AJ4" s="76"/>
+      <c r="AK4" s="76"/>
+      <c r="AL4" s="76"/>
+      <c r="AM4" s="76"/>
+      <c r="AN4" s="76"/>
+      <c r="AO4" s="76"/>
+      <c r="AP4" s="76"/>
+      <c r="AQ4" s="76"/>
+      <c r="AR4" s="76"/>
+      <c r="AS4" s="76"/>
+      <c r="AT4" s="76"/>
+      <c r="AU4" s="76"/>
+      <c r="AV4" s="76"/>
+      <c r="AW4" s="76"/>
+      <c r="AX4" s="76"/>
+      <c r="AY4" s="76"/>
+      <c r="AZ4" s="76"/>
+      <c r="BA4" s="77"/>
     </row>
     <row r="5" spans="1:61">
       <c r="A5" s="27">
@@ -3614,14 +3620,14 @@
       <c r="J5" s="32"/>
       <c r="K5" s="32"/>
       <c r="L5" s="33"/>
-      <c r="M5" s="75" t="s">
+      <c r="M5" s="72" t="s">
         <v>43</v>
       </c>
-      <c r="N5" s="76"/>
-      <c r="O5" s="76"/>
-      <c r="P5" s="76"/>
-      <c r="Q5" s="76"/>
-      <c r="R5" s="77"/>
+      <c r="N5" s="73"/>
+      <c r="O5" s="73"/>
+      <c r="P5" s="73"/>
+      <c r="Q5" s="73"/>
+      <c r="R5" s="74"/>
       <c r="S5" s="31" t="s">
         <v>3</v>
       </c>
@@ -3681,14 +3687,14 @@
       <c r="J6" s="32"/>
       <c r="K6" s="32"/>
       <c r="L6" s="33"/>
-      <c r="M6" s="75" t="s">
+      <c r="M6" s="72" t="s">
         <v>43</v>
       </c>
-      <c r="N6" s="76"/>
-      <c r="O6" s="76"/>
-      <c r="P6" s="76"/>
-      <c r="Q6" s="76"/>
-      <c r="R6" s="77"/>
+      <c r="N6" s="73"/>
+      <c r="O6" s="73"/>
+      <c r="P6" s="73"/>
+      <c r="Q6" s="73"/>
+      <c r="R6" s="74"/>
       <c r="S6" s="31" t="s">
         <v>3</v>
       </c>
@@ -3752,14 +3758,14 @@
       <c r="J7" s="32"/>
       <c r="K7" s="32"/>
       <c r="L7" s="33"/>
-      <c r="M7" s="75" t="s">
+      <c r="M7" s="72" t="s">
         <v>44</v>
       </c>
-      <c r="N7" s="76"/>
-      <c r="O7" s="76"/>
-      <c r="P7" s="76"/>
-      <c r="Q7" s="76"/>
-      <c r="R7" s="77"/>
+      <c r="N7" s="73"/>
+      <c r="O7" s="73"/>
+      <c r="P7" s="73"/>
+      <c r="Q7" s="73"/>
+      <c r="R7" s="74"/>
       <c r="S7" s="31" t="s">
         <v>3</v>
       </c>
@@ -3816,14 +3822,14 @@
       <c r="J8" s="29"/>
       <c r="K8" s="29"/>
       <c r="L8" s="30"/>
-      <c r="M8" s="75" t="s">
+      <c r="M8" s="72" t="s">
         <v>43</v>
       </c>
-      <c r="N8" s="76"/>
-      <c r="O8" s="76"/>
-      <c r="P8" s="76"/>
-      <c r="Q8" s="76"/>
-      <c r="R8" s="77"/>
+      <c r="N8" s="73"/>
+      <c r="O8" s="73"/>
+      <c r="P8" s="73"/>
+      <c r="Q8" s="73"/>
+      <c r="R8" s="74"/>
       <c r="S8" s="31" t="s">
         <v>41</v>
       </c>
@@ -3880,14 +3886,14 @@
       <c r="J9" s="32"/>
       <c r="K9" s="32"/>
       <c r="L9" s="33"/>
-      <c r="M9" s="75" t="s">
+      <c r="M9" s="72" t="s">
         <v>43</v>
       </c>
-      <c r="N9" s="76"/>
-      <c r="O9" s="76"/>
-      <c r="P9" s="76"/>
-      <c r="Q9" s="76"/>
-      <c r="R9" s="77"/>
+      <c r="N9" s="73"/>
+      <c r="O9" s="73"/>
+      <c r="P9" s="73"/>
+      <c r="Q9" s="73"/>
+      <c r="R9" s="74"/>
       <c r="S9" s="31" t="s">
         <v>41</v>
       </c>
@@ -3944,14 +3950,14 @@
       <c r="J10" s="29"/>
       <c r="K10" s="29"/>
       <c r="L10" s="30"/>
-      <c r="M10" s="75" t="s">
+      <c r="M10" s="72" t="s">
         <v>43</v>
       </c>
-      <c r="N10" s="76"/>
-      <c r="O10" s="76"/>
-      <c r="P10" s="76"/>
-      <c r="Q10" s="76"/>
-      <c r="R10" s="77"/>
+      <c r="N10" s="73"/>
+      <c r="O10" s="73"/>
+      <c r="P10" s="73"/>
+      <c r="Q10" s="73"/>
+      <c r="R10" s="74"/>
       <c r="S10" s="31" t="s">
         <v>41</v>
       </c>
@@ -4008,14 +4014,14 @@
       <c r="J11" s="29"/>
       <c r="K11" s="29"/>
       <c r="L11" s="30"/>
-      <c r="M11" s="75" t="s">
+      <c r="M11" s="72" t="s">
         <v>44</v>
       </c>
-      <c r="N11" s="76"/>
-      <c r="O11" s="76"/>
-      <c r="P11" s="76"/>
-      <c r="Q11" s="76"/>
-      <c r="R11" s="77"/>
+      <c r="N11" s="73"/>
+      <c r="O11" s="73"/>
+      <c r="P11" s="73"/>
+      <c r="Q11" s="73"/>
+      <c r="R11" s="74"/>
       <c r="S11" s="31" t="s">
         <v>41</v>
       </c>
@@ -4072,14 +4078,14 @@
       <c r="J12" s="29"/>
       <c r="K12" s="29"/>
       <c r="L12" s="30"/>
-      <c r="M12" s="75" t="s">
+      <c r="M12" s="72" t="s">
         <v>43</v>
       </c>
-      <c r="N12" s="76"/>
-      <c r="O12" s="76"/>
-      <c r="P12" s="76"/>
-      <c r="Q12" s="76"/>
-      <c r="R12" s="77"/>
+      <c r="N12" s="73"/>
+      <c r="O12" s="73"/>
+      <c r="P12" s="73"/>
+      <c r="Q12" s="73"/>
+      <c r="R12" s="74"/>
       <c r="S12" s="31" t="s">
         <v>42</v>
       </c>
@@ -4136,14 +4142,14 @@
       <c r="J13" s="29"/>
       <c r="K13" s="29"/>
       <c r="L13" s="30"/>
-      <c r="M13" s="75" t="s">
+      <c r="M13" s="72" t="s">
         <v>43</v>
       </c>
-      <c r="N13" s="76"/>
-      <c r="O13" s="76"/>
-      <c r="P13" s="76"/>
-      <c r="Q13" s="76"/>
-      <c r="R13" s="77"/>
+      <c r="N13" s="73"/>
+      <c r="O13" s="73"/>
+      <c r="P13" s="73"/>
+      <c r="Q13" s="73"/>
+      <c r="R13" s="74"/>
       <c r="S13" s="31" t="s">
         <v>42</v>
       </c>
@@ -4200,14 +4206,14 @@
       <c r="J14" s="29"/>
       <c r="K14" s="29"/>
       <c r="L14" s="30"/>
-      <c r="M14" s="75" t="s">
+      <c r="M14" s="72" t="s">
         <v>43</v>
       </c>
-      <c r="N14" s="76"/>
-      <c r="O14" s="76"/>
-      <c r="P14" s="76"/>
-      <c r="Q14" s="76"/>
-      <c r="R14" s="77"/>
+      <c r="N14" s="73"/>
+      <c r="O14" s="73"/>
+      <c r="P14" s="73"/>
+      <c r="Q14" s="73"/>
+      <c r="R14" s="74"/>
       <c r="S14" s="31" t="s">
         <v>42</v>
       </c>
@@ -4264,14 +4270,14 @@
       <c r="J15" s="29"/>
       <c r="K15" s="29"/>
       <c r="L15" s="30"/>
-      <c r="M15" s="75" t="s">
+      <c r="M15" s="72" t="s">
         <v>44</v>
       </c>
-      <c r="N15" s="76"/>
-      <c r="O15" s="76"/>
-      <c r="P15" s="76"/>
-      <c r="Q15" s="76"/>
-      <c r="R15" s="77"/>
+      <c r="N15" s="73"/>
+      <c r="O15" s="73"/>
+      <c r="P15" s="73"/>
+      <c r="Q15" s="73"/>
+      <c r="R15" s="74"/>
       <c r="S15" s="31"/>
       <c r="T15" s="32"/>
       <c r="U15" s="32"/>
@@ -4324,14 +4330,14 @@
       <c r="J16" s="29"/>
       <c r="K16" s="29"/>
       <c r="L16" s="30"/>
-      <c r="M16" s="75" t="s">
+      <c r="M16" s="72" t="s">
         <v>17</v>
       </c>
-      <c r="N16" s="76"/>
-      <c r="O16" s="76"/>
-      <c r="P16" s="76"/>
-      <c r="Q16" s="76"/>
-      <c r="R16" s="77"/>
+      <c r="N16" s="73"/>
+      <c r="O16" s="73"/>
+      <c r="P16" s="73"/>
+      <c r="Q16" s="73"/>
+      <c r="R16" s="74"/>
       <c r="S16" s="31"/>
       <c r="T16" s="32"/>
       <c r="U16" s="32"/>
@@ -4370,6 +4376,16 @@
     </row>
   </sheetData>
   <mergeCells count="22">
+    <mergeCell ref="A1:O1"/>
+    <mergeCell ref="M8:R8"/>
+    <mergeCell ref="M9:R9"/>
+    <mergeCell ref="M10:R10"/>
+    <mergeCell ref="M11:R11"/>
+    <mergeCell ref="AI1:AM1"/>
+    <mergeCell ref="AI2:AM2"/>
+    <mergeCell ref="AN1:BA1"/>
+    <mergeCell ref="AN2:BA2"/>
+    <mergeCell ref="P1:AH1"/>
     <mergeCell ref="M16:R16"/>
     <mergeCell ref="S4:BA4"/>
     <mergeCell ref="A3:G3"/>
@@ -4382,16 +4398,6 @@
     <mergeCell ref="M5:R5"/>
     <mergeCell ref="M6:R6"/>
     <mergeCell ref="M7:R7"/>
-    <mergeCell ref="AI1:AM1"/>
-    <mergeCell ref="AI2:AM2"/>
-    <mergeCell ref="AN1:BA1"/>
-    <mergeCell ref="AN2:BA2"/>
-    <mergeCell ref="P1:AH1"/>
-    <mergeCell ref="A1:O1"/>
-    <mergeCell ref="M8:R8"/>
-    <mergeCell ref="M9:R9"/>
-    <mergeCell ref="M10:R10"/>
-    <mergeCell ref="M11:R11"/>
   </mergeCells>
   <dataValidations count="1">
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="M5:R16">
@@ -4399,7 +4405,7 @@
     </dataValidation>
   </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="0" orientation="portrait" horizontalDpi="0" verticalDpi="0" copies="0"/>
+  <pageSetup orientation="portrait" horizontalDpi="200" verticalDpi="200" copies="0" r:id="rId1"/>
   <headerFooter>
     <oddHeader>&amp;CSPECIFY USE CASE</oddHeader>
   </headerFooter>
@@ -4411,8 +4417,8 @@
   <sheetPr codeName="Sheet4"/>
   <dimension ref="A1:BA266"/>
   <sheetViews>
-    <sheetView tabSelected="1" view="pageBreakPreview" topLeftCell="A8" zoomScaleNormal="100" zoomScaleSheetLayoutView="100" workbookViewId="0">
-      <selection activeCell="B27" sqref="B27"/>
+    <sheetView tabSelected="1" view="pageBreakPreview" topLeftCell="A52" zoomScaleNormal="100" zoomScaleSheetLayoutView="100" workbookViewId="0">
+      <selection activeCell="Q65" sqref="Q65:BA65"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -4423,69 +4429,69 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:53">
-      <c r="A1" s="94" t="s">
+      <c r="A1" s="102" t="s">
         <v>4</v>
       </c>
-      <c r="B1" s="95"/>
-      <c r="C1" s="95"/>
-      <c r="D1" s="95"/>
-      <c r="E1" s="95"/>
-      <c r="F1" s="95"/>
-      <c r="G1" s="95"/>
-      <c r="H1" s="95"/>
-      <c r="I1" s="95"/>
-      <c r="J1" s="95"/>
-      <c r="K1" s="95"/>
-      <c r="L1" s="95"/>
-      <c r="M1" s="95"/>
-      <c r="N1" s="95"/>
-      <c r="O1" s="96"/>
-      <c r="P1" s="97" t="str">
+      <c r="B1" s="103"/>
+      <c r="C1" s="103"/>
+      <c r="D1" s="103"/>
+      <c r="E1" s="103"/>
+      <c r="F1" s="103"/>
+      <c r="G1" s="103"/>
+      <c r="H1" s="103"/>
+      <c r="I1" s="103"/>
+      <c r="J1" s="103"/>
+      <c r="K1" s="103"/>
+      <c r="L1" s="103"/>
+      <c r="M1" s="103"/>
+      <c r="N1" s="103"/>
+      <c r="O1" s="104"/>
+      <c r="P1" s="105" t="str">
         <f>'History(Lich Su)'!A4</f>
         <v>Quản Lý Giải Vô Địch Bóng Đá Quốc Gia</v>
       </c>
-      <c r="Q1" s="97"/>
-      <c r="R1" s="97"/>
-      <c r="S1" s="97"/>
-      <c r="T1" s="97"/>
-      <c r="U1" s="97"/>
-      <c r="V1" s="97"/>
-      <c r="W1" s="97"/>
-      <c r="X1" s="97"/>
-      <c r="Y1" s="97"/>
-      <c r="Z1" s="97"/>
-      <c r="AA1" s="97"/>
-      <c r="AB1" s="97"/>
-      <c r="AC1" s="97"/>
-      <c r="AD1" s="97"/>
-      <c r="AE1" s="97"/>
-      <c r="AF1" s="97"/>
-      <c r="AG1" s="97"/>
-      <c r="AH1" s="98"/>
-      <c r="AI1" s="99" t="s">
+      <c r="Q1" s="105"/>
+      <c r="R1" s="105"/>
+      <c r="S1" s="105"/>
+      <c r="T1" s="105"/>
+      <c r="U1" s="105"/>
+      <c r="V1" s="105"/>
+      <c r="W1" s="105"/>
+      <c r="X1" s="105"/>
+      <c r="Y1" s="105"/>
+      <c r="Z1" s="105"/>
+      <c r="AA1" s="105"/>
+      <c r="AB1" s="105"/>
+      <c r="AC1" s="105"/>
+      <c r="AD1" s="105"/>
+      <c r="AE1" s="105"/>
+      <c r="AF1" s="105"/>
+      <c r="AG1" s="105"/>
+      <c r="AH1" s="106"/>
+      <c r="AI1" s="107" t="s">
         <v>1</v>
       </c>
-      <c r="AJ1" s="100"/>
-      <c r="AK1" s="100"/>
-      <c r="AL1" s="100"/>
-      <c r="AM1" s="101"/>
-      <c r="AN1" s="102">
+      <c r="AJ1" s="108"/>
+      <c r="AK1" s="108"/>
+      <c r="AL1" s="108"/>
+      <c r="AM1" s="109"/>
+      <c r="AN1" s="110">
         <f>'History(Lich Su)'!C6</f>
         <v>40997</v>
       </c>
-      <c r="AO1" s="103"/>
-      <c r="AP1" s="103"/>
-      <c r="AQ1" s="103"/>
-      <c r="AR1" s="103"/>
-      <c r="AS1" s="103"/>
-      <c r="AT1" s="103"/>
-      <c r="AU1" s="103"/>
-      <c r="AV1" s="103"/>
-      <c r="AW1" s="103"/>
-      <c r="AX1" s="103"/>
-      <c r="AY1" s="103"/>
-      <c r="AZ1" s="103"/>
-      <c r="BA1" s="104"/>
+      <c r="AO1" s="111"/>
+      <c r="AP1" s="111"/>
+      <c r="AQ1" s="111"/>
+      <c r="AR1" s="111"/>
+      <c r="AS1" s="111"/>
+      <c r="AT1" s="111"/>
+      <c r="AU1" s="111"/>
+      <c r="AV1" s="111"/>
+      <c r="AW1" s="111"/>
+      <c r="AX1" s="111"/>
+      <c r="AY1" s="111"/>
+      <c r="AZ1" s="111"/>
+      <c r="BA1" s="112"/>
     </row>
     <row r="2" spans="1:53">
       <c r="A2" s="19"/>
@@ -4522,42 +4528,42 @@
       <c r="AF2" s="18"/>
       <c r="AG2" s="18"/>
       <c r="AH2" s="20"/>
-      <c r="AI2" s="94" t="s">
+      <c r="AI2" s="102" t="s">
         <v>2</v>
       </c>
-      <c r="AJ2" s="95"/>
-      <c r="AK2" s="95"/>
-      <c r="AL2" s="95"/>
-      <c r="AM2" s="96"/>
-      <c r="AN2" s="105" t="str">
+      <c r="AJ2" s="103"/>
+      <c r="AK2" s="103"/>
+      <c r="AL2" s="103"/>
+      <c r="AM2" s="104"/>
+      <c r="AN2" s="113" t="str">
         <f>'History(Lich Su)'!AS6</f>
         <v>HaiPM</v>
       </c>
-      <c r="AO2" s="103"/>
-      <c r="AP2" s="103"/>
-      <c r="AQ2" s="103"/>
-      <c r="AR2" s="103"/>
-      <c r="AS2" s="103"/>
-      <c r="AT2" s="103"/>
-      <c r="AU2" s="103"/>
-      <c r="AV2" s="103"/>
-      <c r="AW2" s="103"/>
-      <c r="AX2" s="103"/>
-      <c r="AY2" s="103"/>
-      <c r="AZ2" s="103"/>
-      <c r="BA2" s="104"/>
+      <c r="AO2" s="111"/>
+      <c r="AP2" s="111"/>
+      <c r="AQ2" s="111"/>
+      <c r="AR2" s="111"/>
+      <c r="AS2" s="111"/>
+      <c r="AT2" s="111"/>
+      <c r="AU2" s="111"/>
+      <c r="AV2" s="111"/>
+      <c r="AW2" s="111"/>
+      <c r="AX2" s="111"/>
+      <c r="AY2" s="111"/>
+      <c r="AZ2" s="111"/>
+      <c r="BA2" s="112"/>
     </row>
     <row r="3" spans="1:53">
-      <c r="A3" s="111" t="s">
+      <c r="A3" s="99" t="s">
         <v>29</v>
       </c>
-      <c r="B3" s="112"/>
-      <c r="C3" s="112"/>
-      <c r="D3" s="112"/>
-      <c r="E3" s="112"/>
-      <c r="F3" s="112"/>
-      <c r="G3" s="112"/>
-      <c r="H3" s="113"/>
+      <c r="B3" s="100"/>
+      <c r="C3" s="100"/>
+      <c r="D3" s="100"/>
+      <c r="E3" s="100"/>
+      <c r="F3" s="100"/>
+      <c r="G3" s="100"/>
+      <c r="H3" s="101"/>
       <c r="I3" s="18" t="str">
         <f>VLOOKUP(B4,'SPECIFY(Đặc Tả)(1)'!$A$5:$BA$33,19,0)</f>
         <v>HaiPM</v>
@@ -4614,62 +4620,62 @@
       <c r="B4" s="17">
         <v>1</v>
       </c>
-      <c r="C4" s="106" t="s">
+      <c r="C4" s="94" t="s">
         <v>30</v>
       </c>
-      <c r="D4" s="107"/>
-      <c r="E4" s="107"/>
-      <c r="F4" s="107"/>
-      <c r="G4" s="107"/>
-      <c r="H4" s="107"/>
-      <c r="I4" s="107"/>
-      <c r="J4" s="107"/>
-      <c r="K4" s="107"/>
-      <c r="L4" s="107"/>
-      <c r="M4" s="107"/>
-      <c r="N4" s="107"/>
-      <c r="O4" s="107"/>
-      <c r="P4" s="108"/>
-      <c r="Q4" s="109" t="str">
+      <c r="D4" s="95"/>
+      <c r="E4" s="95"/>
+      <c r="F4" s="95"/>
+      <c r="G4" s="95"/>
+      <c r="H4" s="95"/>
+      <c r="I4" s="95"/>
+      <c r="J4" s="95"/>
+      <c r="K4" s="95"/>
+      <c r="L4" s="95"/>
+      <c r="M4" s="95"/>
+      <c r="N4" s="95"/>
+      <c r="O4" s="95"/>
+      <c r="P4" s="96"/>
+      <c r="Q4" s="114" t="str">
         <f>VLOOKUP(B4,'SPECIFY(Đặc Tả)(1)'!$A$5:$BA$33,2,0)</f>
         <v>Tiếp nhận HS các đội đăng ký mới</v>
       </c>
-      <c r="R4" s="110"/>
-      <c r="S4" s="110"/>
-      <c r="T4" s="110"/>
-      <c r="U4" s="110"/>
-      <c r="V4" s="110"/>
-      <c r="W4" s="110"/>
-      <c r="X4" s="110"/>
-      <c r="Y4" s="110"/>
-      <c r="Z4" s="110"/>
-      <c r="AA4" s="110"/>
-      <c r="AB4" s="110"/>
-      <c r="AC4" s="110"/>
-      <c r="AD4" s="110"/>
-      <c r="AE4" s="110"/>
-      <c r="AF4" s="110"/>
-      <c r="AG4" s="110"/>
-      <c r="AH4" s="110"/>
-      <c r="AI4" s="110"/>
-      <c r="AJ4" s="110"/>
-      <c r="AK4" s="110"/>
-      <c r="AL4" s="110"/>
-      <c r="AM4" s="110"/>
-      <c r="AN4" s="110"/>
-      <c r="AO4" s="110"/>
-      <c r="AP4" s="110"/>
-      <c r="AQ4" s="110"/>
-      <c r="AR4" s="110"/>
-      <c r="AS4" s="110"/>
-      <c r="AT4" s="110"/>
-      <c r="AU4" s="110"/>
-      <c r="AV4" s="110"/>
-      <c r="AW4" s="110"/>
-      <c r="AX4" s="110"/>
-      <c r="AY4" s="110"/>
-      <c r="AZ4" s="110"/>
-      <c r="BA4" s="110"/>
+      <c r="R4" s="115"/>
+      <c r="S4" s="115"/>
+      <c r="T4" s="115"/>
+      <c r="U4" s="115"/>
+      <c r="V4" s="115"/>
+      <c r="W4" s="115"/>
+      <c r="X4" s="115"/>
+      <c r="Y4" s="115"/>
+      <c r="Z4" s="115"/>
+      <c r="AA4" s="115"/>
+      <c r="AB4" s="115"/>
+      <c r="AC4" s="115"/>
+      <c r="AD4" s="115"/>
+      <c r="AE4" s="115"/>
+      <c r="AF4" s="115"/>
+      <c r="AG4" s="115"/>
+      <c r="AH4" s="115"/>
+      <c r="AI4" s="115"/>
+      <c r="AJ4" s="115"/>
+      <c r="AK4" s="115"/>
+      <c r="AL4" s="115"/>
+      <c r="AM4" s="115"/>
+      <c r="AN4" s="115"/>
+      <c r="AO4" s="115"/>
+      <c r="AP4" s="115"/>
+      <c r="AQ4" s="115"/>
+      <c r="AR4" s="115"/>
+      <c r="AS4" s="115"/>
+      <c r="AT4" s="115"/>
+      <c r="AU4" s="115"/>
+      <c r="AV4" s="115"/>
+      <c r="AW4" s="115"/>
+      <c r="AX4" s="115"/>
+      <c r="AY4" s="115"/>
+      <c r="AZ4" s="115"/>
+      <c r="BA4" s="115"/>
     </row>
     <row r="5" spans="1:53">
       <c r="A5" s="51" t="s">
@@ -5882,62 +5888,62 @@
       <c r="B26" s="17">
         <v>2</v>
       </c>
-      <c r="C26" s="106" t="s">
+      <c r="C26" s="94" t="s">
         <v>30</v>
       </c>
-      <c r="D26" s="107"/>
-      <c r="E26" s="107"/>
-      <c r="F26" s="107"/>
-      <c r="G26" s="107"/>
-      <c r="H26" s="107"/>
-      <c r="I26" s="107"/>
-      <c r="J26" s="107"/>
-      <c r="K26" s="107"/>
-      <c r="L26" s="107"/>
-      <c r="M26" s="107"/>
-      <c r="N26" s="107"/>
-      <c r="O26" s="107"/>
-      <c r="P26" s="108"/>
-      <c r="Q26" s="109" t="str">
+      <c r="D26" s="95"/>
+      <c r="E26" s="95"/>
+      <c r="F26" s="95"/>
+      <c r="G26" s="95"/>
+      <c r="H26" s="95"/>
+      <c r="I26" s="95"/>
+      <c r="J26" s="95"/>
+      <c r="K26" s="95"/>
+      <c r="L26" s="95"/>
+      <c r="M26" s="95"/>
+      <c r="N26" s="95"/>
+      <c r="O26" s="95"/>
+      <c r="P26" s="96"/>
+      <c r="Q26" s="114" t="str">
         <f>VLOOKUP(B26,'SPECIFY(Đặc Tả)(1)'!$A$5:$BA$33,2,0)</f>
         <v>Tiếp nhận DS các cầu thủ</v>
       </c>
-      <c r="R26" s="110"/>
-      <c r="S26" s="110"/>
-      <c r="T26" s="110"/>
-      <c r="U26" s="110"/>
-      <c r="V26" s="110"/>
-      <c r="W26" s="110"/>
-      <c r="X26" s="110"/>
-      <c r="Y26" s="110"/>
-      <c r="Z26" s="110"/>
-      <c r="AA26" s="110"/>
-      <c r="AB26" s="110"/>
-      <c r="AC26" s="110"/>
-      <c r="AD26" s="110"/>
-      <c r="AE26" s="110"/>
-      <c r="AF26" s="110"/>
-      <c r="AG26" s="110"/>
-      <c r="AH26" s="110"/>
-      <c r="AI26" s="110"/>
-      <c r="AJ26" s="110"/>
-      <c r="AK26" s="110"/>
-      <c r="AL26" s="110"/>
-      <c r="AM26" s="110"/>
-      <c r="AN26" s="110"/>
-      <c r="AO26" s="110"/>
-      <c r="AP26" s="110"/>
-      <c r="AQ26" s="110"/>
-      <c r="AR26" s="110"/>
-      <c r="AS26" s="110"/>
-      <c r="AT26" s="110"/>
-      <c r="AU26" s="110"/>
-      <c r="AV26" s="110"/>
-      <c r="AW26" s="110"/>
-      <c r="AX26" s="110"/>
-      <c r="AY26" s="110"/>
-      <c r="AZ26" s="110"/>
-      <c r="BA26" s="110"/>
+      <c r="R26" s="115"/>
+      <c r="S26" s="115"/>
+      <c r="T26" s="115"/>
+      <c r="U26" s="115"/>
+      <c r="V26" s="115"/>
+      <c r="W26" s="115"/>
+      <c r="X26" s="115"/>
+      <c r="Y26" s="115"/>
+      <c r="Z26" s="115"/>
+      <c r="AA26" s="115"/>
+      <c r="AB26" s="115"/>
+      <c r="AC26" s="115"/>
+      <c r="AD26" s="115"/>
+      <c r="AE26" s="115"/>
+      <c r="AF26" s="115"/>
+      <c r="AG26" s="115"/>
+      <c r="AH26" s="115"/>
+      <c r="AI26" s="115"/>
+      <c r="AJ26" s="115"/>
+      <c r="AK26" s="115"/>
+      <c r="AL26" s="115"/>
+      <c r="AM26" s="115"/>
+      <c r="AN26" s="115"/>
+      <c r="AO26" s="115"/>
+      <c r="AP26" s="115"/>
+      <c r="AQ26" s="115"/>
+      <c r="AR26" s="115"/>
+      <c r="AS26" s="115"/>
+      <c r="AT26" s="115"/>
+      <c r="AU26" s="115"/>
+      <c r="AV26" s="115"/>
+      <c r="AW26" s="115"/>
+      <c r="AX26" s="115"/>
+      <c r="AY26" s="115"/>
+      <c r="AZ26" s="115"/>
+      <c r="BA26" s="115"/>
     </row>
     <row r="27" spans="1:53">
       <c r="A27" s="51" t="s">
@@ -6693,62 +6699,62 @@
       <c r="B40" s="17">
         <v>3</v>
       </c>
-      <c r="C40" s="106" t="s">
+      <c r="C40" s="94" t="s">
         <v>30</v>
       </c>
-      <c r="D40" s="107"/>
-      <c r="E40" s="107"/>
-      <c r="F40" s="107"/>
-      <c r="G40" s="107"/>
-      <c r="H40" s="107"/>
-      <c r="I40" s="107"/>
-      <c r="J40" s="107"/>
-      <c r="K40" s="107"/>
-      <c r="L40" s="107"/>
-      <c r="M40" s="107"/>
-      <c r="N40" s="107"/>
-      <c r="O40" s="107"/>
-      <c r="P40" s="108"/>
-      <c r="Q40" s="109" t="str">
+      <c r="D40" s="95"/>
+      <c r="E40" s="95"/>
+      <c r="F40" s="95"/>
+      <c r="G40" s="95"/>
+      <c r="H40" s="95"/>
+      <c r="I40" s="95"/>
+      <c r="J40" s="95"/>
+      <c r="K40" s="95"/>
+      <c r="L40" s="95"/>
+      <c r="M40" s="95"/>
+      <c r="N40" s="95"/>
+      <c r="O40" s="95"/>
+      <c r="P40" s="96"/>
+      <c r="Q40" s="114" t="str">
         <f>VLOOKUP(B40,'SPECIFY(Đặc Tả)(1)'!$A$5:$BA$33,2,0)</f>
         <v>Lập lịch thi đấu</v>
       </c>
-      <c r="R40" s="110"/>
-      <c r="S40" s="110"/>
-      <c r="T40" s="110"/>
-      <c r="U40" s="110"/>
-      <c r="V40" s="110"/>
-      <c r="W40" s="110"/>
-      <c r="X40" s="110"/>
-      <c r="Y40" s="110"/>
-      <c r="Z40" s="110"/>
-      <c r="AA40" s="110"/>
-      <c r="AB40" s="110"/>
-      <c r="AC40" s="110"/>
-      <c r="AD40" s="110"/>
-      <c r="AE40" s="110"/>
-      <c r="AF40" s="110"/>
-      <c r="AG40" s="110"/>
-      <c r="AH40" s="110"/>
-      <c r="AI40" s="110"/>
-      <c r="AJ40" s="110"/>
-      <c r="AK40" s="110"/>
-      <c r="AL40" s="110"/>
-      <c r="AM40" s="110"/>
-      <c r="AN40" s="110"/>
-      <c r="AO40" s="110"/>
-      <c r="AP40" s="110"/>
-      <c r="AQ40" s="110"/>
-      <c r="AR40" s="110"/>
-      <c r="AS40" s="110"/>
-      <c r="AT40" s="110"/>
-      <c r="AU40" s="110"/>
-      <c r="AV40" s="110"/>
-      <c r="AW40" s="110"/>
-      <c r="AX40" s="110"/>
-      <c r="AY40" s="110"/>
-      <c r="AZ40" s="110"/>
-      <c r="BA40" s="110"/>
+      <c r="R40" s="115"/>
+      <c r="S40" s="115"/>
+      <c r="T40" s="115"/>
+      <c r="U40" s="115"/>
+      <c r="V40" s="115"/>
+      <c r="W40" s="115"/>
+      <c r="X40" s="115"/>
+      <c r="Y40" s="115"/>
+      <c r="Z40" s="115"/>
+      <c r="AA40" s="115"/>
+      <c r="AB40" s="115"/>
+      <c r="AC40" s="115"/>
+      <c r="AD40" s="115"/>
+      <c r="AE40" s="115"/>
+      <c r="AF40" s="115"/>
+      <c r="AG40" s="115"/>
+      <c r="AH40" s="115"/>
+      <c r="AI40" s="115"/>
+      <c r="AJ40" s="115"/>
+      <c r="AK40" s="115"/>
+      <c r="AL40" s="115"/>
+      <c r="AM40" s="115"/>
+      <c r="AN40" s="115"/>
+      <c r="AO40" s="115"/>
+      <c r="AP40" s="115"/>
+      <c r="AQ40" s="115"/>
+      <c r="AR40" s="115"/>
+      <c r="AS40" s="115"/>
+      <c r="AT40" s="115"/>
+      <c r="AU40" s="115"/>
+      <c r="AV40" s="115"/>
+      <c r="AW40" s="115"/>
+      <c r="AX40" s="115"/>
+      <c r="AY40" s="115"/>
+      <c r="AZ40" s="115"/>
+      <c r="BA40" s="115"/>
     </row>
     <row r="41" spans="1:53">
       <c r="A41" s="51" t="s">
@@ -8098,62 +8104,62 @@
       <c r="B65" s="17">
         <v>4</v>
       </c>
-      <c r="C65" s="106" t="s">
+      <c r="C65" s="94" t="s">
         <v>30</v>
       </c>
-      <c r="D65" s="107"/>
-      <c r="E65" s="107"/>
-      <c r="F65" s="107"/>
-      <c r="G65" s="107"/>
-      <c r="H65" s="107"/>
-      <c r="I65" s="107"/>
-      <c r="J65" s="107"/>
-      <c r="K65" s="107"/>
-      <c r="L65" s="107"/>
-      <c r="M65" s="107"/>
-      <c r="N65" s="107"/>
-      <c r="O65" s="107"/>
-      <c r="P65" s="108"/>
-      <c r="Q65" s="109" t="str">
+      <c r="D65" s="95"/>
+      <c r="E65" s="95"/>
+      <c r="F65" s="95"/>
+      <c r="G65" s="95"/>
+      <c r="H65" s="95"/>
+      <c r="I65" s="95"/>
+      <c r="J65" s="95"/>
+      <c r="K65" s="95"/>
+      <c r="L65" s="95"/>
+      <c r="M65" s="95"/>
+      <c r="N65" s="95"/>
+      <c r="O65" s="95"/>
+      <c r="P65" s="96"/>
+      <c r="Q65" s="114" t="str">
         <f>VLOOKUP(B65,'SPECIFY(Đặc Tả)(1)'!$A$5:$BA$33,2,0)</f>
         <v>Ghi nhận KQ trận đấu</v>
       </c>
-      <c r="R65" s="110"/>
-      <c r="S65" s="110"/>
-      <c r="T65" s="110"/>
-      <c r="U65" s="110"/>
-      <c r="V65" s="110"/>
-      <c r="W65" s="110"/>
-      <c r="X65" s="110"/>
-      <c r="Y65" s="110"/>
-      <c r="Z65" s="110"/>
-      <c r="AA65" s="110"/>
-      <c r="AB65" s="110"/>
-      <c r="AC65" s="110"/>
-      <c r="AD65" s="110"/>
-      <c r="AE65" s="110"/>
-      <c r="AF65" s="110"/>
-      <c r="AG65" s="110"/>
-      <c r="AH65" s="110"/>
-      <c r="AI65" s="110"/>
-      <c r="AJ65" s="110"/>
-      <c r="AK65" s="110"/>
-      <c r="AL65" s="110"/>
-      <c r="AM65" s="110"/>
-      <c r="AN65" s="110"/>
-      <c r="AO65" s="110"/>
-      <c r="AP65" s="110"/>
-      <c r="AQ65" s="110"/>
-      <c r="AR65" s="110"/>
-      <c r="AS65" s="110"/>
-      <c r="AT65" s="110"/>
-      <c r="AU65" s="110"/>
-      <c r="AV65" s="110"/>
-      <c r="AW65" s="110"/>
-      <c r="AX65" s="110"/>
-      <c r="AY65" s="110"/>
-      <c r="AZ65" s="110"/>
-      <c r="BA65" s="110"/>
+      <c r="R65" s="115"/>
+      <c r="S65" s="115"/>
+      <c r="T65" s="115"/>
+      <c r="U65" s="115"/>
+      <c r="V65" s="115"/>
+      <c r="W65" s="115"/>
+      <c r="X65" s="115"/>
+      <c r="Y65" s="115"/>
+      <c r="Z65" s="115"/>
+      <c r="AA65" s="115"/>
+      <c r="AB65" s="115"/>
+      <c r="AC65" s="115"/>
+      <c r="AD65" s="115"/>
+      <c r="AE65" s="115"/>
+      <c r="AF65" s="115"/>
+      <c r="AG65" s="115"/>
+      <c r="AH65" s="115"/>
+      <c r="AI65" s="115"/>
+      <c r="AJ65" s="115"/>
+      <c r="AK65" s="115"/>
+      <c r="AL65" s="115"/>
+      <c r="AM65" s="115"/>
+      <c r="AN65" s="115"/>
+      <c r="AO65" s="115"/>
+      <c r="AP65" s="115"/>
+      <c r="AQ65" s="115"/>
+      <c r="AR65" s="115"/>
+      <c r="AS65" s="115"/>
+      <c r="AT65" s="115"/>
+      <c r="AU65" s="115"/>
+      <c r="AV65" s="115"/>
+      <c r="AW65" s="115"/>
+      <c r="AX65" s="115"/>
+      <c r="AY65" s="115"/>
+      <c r="AZ65" s="115"/>
+      <c r="BA65" s="115"/>
     </row>
     <row r="66" spans="1:53">
       <c r="A66" s="51" t="s">
@@ -9546,62 +9552,62 @@
       <c r="B91" s="17">
         <v>5</v>
       </c>
-      <c r="C91" s="106" t="s">
+      <c r="C91" s="94" t="s">
         <v>30</v>
       </c>
-      <c r="D91" s="107"/>
-      <c r="E91" s="107"/>
-      <c r="F91" s="107"/>
-      <c r="G91" s="107"/>
-      <c r="H91" s="107"/>
-      <c r="I91" s="107"/>
-      <c r="J91" s="107"/>
-      <c r="K91" s="107"/>
-      <c r="L91" s="107"/>
-      <c r="M91" s="107"/>
-      <c r="N91" s="107"/>
-      <c r="O91" s="107"/>
-      <c r="P91" s="108"/>
-      <c r="Q91" s="109" t="str">
+      <c r="D91" s="95"/>
+      <c r="E91" s="95"/>
+      <c r="F91" s="95"/>
+      <c r="G91" s="95"/>
+      <c r="H91" s="95"/>
+      <c r="I91" s="95"/>
+      <c r="J91" s="95"/>
+      <c r="K91" s="95"/>
+      <c r="L91" s="95"/>
+      <c r="M91" s="95"/>
+      <c r="N91" s="95"/>
+      <c r="O91" s="95"/>
+      <c r="P91" s="96"/>
+      <c r="Q91" s="97" t="str">
         <f>VLOOKUP(B91,'SPECIFY(Đặc Tả)(1)'!$A$5:$BA$33,2,0)</f>
         <v>Tra cứu cầu thủ</v>
       </c>
-      <c r="R91" s="110"/>
-      <c r="S91" s="110"/>
-      <c r="T91" s="110"/>
-      <c r="U91" s="110"/>
-      <c r="V91" s="110"/>
-      <c r="W91" s="110"/>
-      <c r="X91" s="110"/>
-      <c r="Y91" s="110"/>
-      <c r="Z91" s="110"/>
-      <c r="AA91" s="110"/>
-      <c r="AB91" s="110"/>
-      <c r="AC91" s="110"/>
-      <c r="AD91" s="110"/>
-      <c r="AE91" s="110"/>
-      <c r="AF91" s="110"/>
-      <c r="AG91" s="110"/>
-      <c r="AH91" s="110"/>
-      <c r="AI91" s="110"/>
-      <c r="AJ91" s="110"/>
-      <c r="AK91" s="110"/>
-      <c r="AL91" s="110"/>
-      <c r="AM91" s="110"/>
-      <c r="AN91" s="110"/>
-      <c r="AO91" s="110"/>
-      <c r="AP91" s="110"/>
-      <c r="AQ91" s="110"/>
-      <c r="AR91" s="110"/>
-      <c r="AS91" s="110"/>
-      <c r="AT91" s="110"/>
-      <c r="AU91" s="110"/>
-      <c r="AV91" s="110"/>
-      <c r="AW91" s="110"/>
-      <c r="AX91" s="110"/>
-      <c r="AY91" s="110"/>
-      <c r="AZ91" s="110"/>
-      <c r="BA91" s="110"/>
+      <c r="R91" s="98"/>
+      <c r="S91" s="98"/>
+      <c r="T91" s="98"/>
+      <c r="U91" s="98"/>
+      <c r="V91" s="98"/>
+      <c r="W91" s="98"/>
+      <c r="X91" s="98"/>
+      <c r="Y91" s="98"/>
+      <c r="Z91" s="98"/>
+      <c r="AA91" s="98"/>
+      <c r="AB91" s="98"/>
+      <c r="AC91" s="98"/>
+      <c r="AD91" s="98"/>
+      <c r="AE91" s="98"/>
+      <c r="AF91" s="98"/>
+      <c r="AG91" s="98"/>
+      <c r="AH91" s="98"/>
+      <c r="AI91" s="98"/>
+      <c r="AJ91" s="98"/>
+      <c r="AK91" s="98"/>
+      <c r="AL91" s="98"/>
+      <c r="AM91" s="98"/>
+      <c r="AN91" s="98"/>
+      <c r="AO91" s="98"/>
+      <c r="AP91" s="98"/>
+      <c r="AQ91" s="98"/>
+      <c r="AR91" s="98"/>
+      <c r="AS91" s="98"/>
+      <c r="AT91" s="98"/>
+      <c r="AU91" s="98"/>
+      <c r="AV91" s="98"/>
+      <c r="AW91" s="98"/>
+      <c r="AX91" s="98"/>
+      <c r="AY91" s="98"/>
+      <c r="AZ91" s="98"/>
+      <c r="BA91" s="98"/>
     </row>
     <row r="92" spans="1:53">
       <c r="A92" s="51" t="s">
@@ -10939,62 +10945,62 @@
       <c r="B116" s="17">
         <v>6</v>
       </c>
-      <c r="C116" s="106" t="s">
+      <c r="C116" s="94" t="s">
         <v>30</v>
       </c>
-      <c r="D116" s="107"/>
-      <c r="E116" s="107"/>
-      <c r="F116" s="107"/>
-      <c r="G116" s="107"/>
-      <c r="H116" s="107"/>
-      <c r="I116" s="107"/>
-      <c r="J116" s="107"/>
-      <c r="K116" s="107"/>
-      <c r="L116" s="107"/>
-      <c r="M116" s="107"/>
-      <c r="N116" s="107"/>
-      <c r="O116" s="107"/>
-      <c r="P116" s="108"/>
-      <c r="Q116" s="109" t="str">
+      <c r="D116" s="95"/>
+      <c r="E116" s="95"/>
+      <c r="F116" s="95"/>
+      <c r="G116" s="95"/>
+      <c r="H116" s="95"/>
+      <c r="I116" s="95"/>
+      <c r="J116" s="95"/>
+      <c r="K116" s="95"/>
+      <c r="L116" s="95"/>
+      <c r="M116" s="95"/>
+      <c r="N116" s="95"/>
+      <c r="O116" s="95"/>
+      <c r="P116" s="96"/>
+      <c r="Q116" s="97" t="str">
         <f>VLOOKUP(B116,'SPECIFY(Đặc Tả)(1)'!$A$5:$BA$33,2,0)</f>
         <v>Tra cứu đội bóng</v>
       </c>
-      <c r="R116" s="110"/>
-      <c r="S116" s="110"/>
-      <c r="T116" s="110"/>
-      <c r="U116" s="110"/>
-      <c r="V116" s="110"/>
-      <c r="W116" s="110"/>
-      <c r="X116" s="110"/>
-      <c r="Y116" s="110"/>
-      <c r="Z116" s="110"/>
-      <c r="AA116" s="110"/>
-      <c r="AB116" s="110"/>
-      <c r="AC116" s="110"/>
-      <c r="AD116" s="110"/>
-      <c r="AE116" s="110"/>
-      <c r="AF116" s="110"/>
-      <c r="AG116" s="110"/>
-      <c r="AH116" s="110"/>
-      <c r="AI116" s="110"/>
-      <c r="AJ116" s="110"/>
-      <c r="AK116" s="110"/>
-      <c r="AL116" s="110"/>
-      <c r="AM116" s="110"/>
-      <c r="AN116" s="110"/>
-      <c r="AO116" s="110"/>
-      <c r="AP116" s="110"/>
-      <c r="AQ116" s="110"/>
-      <c r="AR116" s="110"/>
-      <c r="AS116" s="110"/>
-      <c r="AT116" s="110"/>
-      <c r="AU116" s="110"/>
-      <c r="AV116" s="110"/>
-      <c r="AW116" s="110"/>
-      <c r="AX116" s="110"/>
-      <c r="AY116" s="110"/>
-      <c r="AZ116" s="110"/>
-      <c r="BA116" s="110"/>
+      <c r="R116" s="98"/>
+      <c r="S116" s="98"/>
+      <c r="T116" s="98"/>
+      <c r="U116" s="98"/>
+      <c r="V116" s="98"/>
+      <c r="W116" s="98"/>
+      <c r="X116" s="98"/>
+      <c r="Y116" s="98"/>
+      <c r="Z116" s="98"/>
+      <c r="AA116" s="98"/>
+      <c r="AB116" s="98"/>
+      <c r="AC116" s="98"/>
+      <c r="AD116" s="98"/>
+      <c r="AE116" s="98"/>
+      <c r="AF116" s="98"/>
+      <c r="AG116" s="98"/>
+      <c r="AH116" s="98"/>
+      <c r="AI116" s="98"/>
+      <c r="AJ116" s="98"/>
+      <c r="AK116" s="98"/>
+      <c r="AL116" s="98"/>
+      <c r="AM116" s="98"/>
+      <c r="AN116" s="98"/>
+      <c r="AO116" s="98"/>
+      <c r="AP116" s="98"/>
+      <c r="AQ116" s="98"/>
+      <c r="AR116" s="98"/>
+      <c r="AS116" s="98"/>
+      <c r="AT116" s="98"/>
+      <c r="AU116" s="98"/>
+      <c r="AV116" s="98"/>
+      <c r="AW116" s="98"/>
+      <c r="AX116" s="98"/>
+      <c r="AY116" s="98"/>
+      <c r="AZ116" s="98"/>
+      <c r="BA116" s="98"/>
     </row>
     <row r="117" spans="1:53">
       <c r="A117" s="51" t="s">
@@ -12332,62 +12338,62 @@
       <c r="B141" s="17">
         <v>7</v>
       </c>
-      <c r="C141" s="106" t="s">
+      <c r="C141" s="94" t="s">
         <v>30</v>
       </c>
-      <c r="D141" s="107"/>
-      <c r="E141" s="107"/>
-      <c r="F141" s="107"/>
-      <c r="G141" s="107"/>
-      <c r="H141" s="107"/>
-      <c r="I141" s="107"/>
-      <c r="J141" s="107"/>
-      <c r="K141" s="107"/>
-      <c r="L141" s="107"/>
-      <c r="M141" s="107"/>
-      <c r="N141" s="107"/>
-      <c r="O141" s="107"/>
-      <c r="P141" s="108"/>
-      <c r="Q141" s="109" t="str">
+      <c r="D141" s="95"/>
+      <c r="E141" s="95"/>
+      <c r="F141" s="95"/>
+      <c r="G141" s="95"/>
+      <c r="H141" s="95"/>
+      <c r="I141" s="95"/>
+      <c r="J141" s="95"/>
+      <c r="K141" s="95"/>
+      <c r="L141" s="95"/>
+      <c r="M141" s="95"/>
+      <c r="N141" s="95"/>
+      <c r="O141" s="95"/>
+      <c r="P141" s="96"/>
+      <c r="Q141" s="97" t="str">
         <f>VLOOKUP(B141,'SPECIFY(Đặc Tả)(1)'!$A$5:$BA$33,2,0)</f>
         <v>Lập báo cáo giải</v>
       </c>
-      <c r="R141" s="110"/>
-      <c r="S141" s="110"/>
-      <c r="T141" s="110"/>
-      <c r="U141" s="110"/>
-      <c r="V141" s="110"/>
-      <c r="W141" s="110"/>
-      <c r="X141" s="110"/>
-      <c r="Y141" s="110"/>
-      <c r="Z141" s="110"/>
-      <c r="AA141" s="110"/>
-      <c r="AB141" s="110"/>
-      <c r="AC141" s="110"/>
-      <c r="AD141" s="110"/>
-      <c r="AE141" s="110"/>
-      <c r="AF141" s="110"/>
-      <c r="AG141" s="110"/>
-      <c r="AH141" s="110"/>
-      <c r="AI141" s="110"/>
-      <c r="AJ141" s="110"/>
-      <c r="AK141" s="110"/>
-      <c r="AL141" s="110"/>
-      <c r="AM141" s="110"/>
-      <c r="AN141" s="110"/>
-      <c r="AO141" s="110"/>
-      <c r="AP141" s="110"/>
-      <c r="AQ141" s="110"/>
-      <c r="AR141" s="110"/>
-      <c r="AS141" s="110"/>
-      <c r="AT141" s="110"/>
-      <c r="AU141" s="110"/>
-      <c r="AV141" s="110"/>
-      <c r="AW141" s="110"/>
-      <c r="AX141" s="110"/>
-      <c r="AY141" s="110"/>
-      <c r="AZ141" s="110"/>
-      <c r="BA141" s="110"/>
+      <c r="R141" s="98"/>
+      <c r="S141" s="98"/>
+      <c r="T141" s="98"/>
+      <c r="U141" s="98"/>
+      <c r="V141" s="98"/>
+      <c r="W141" s="98"/>
+      <c r="X141" s="98"/>
+      <c r="Y141" s="98"/>
+      <c r="Z141" s="98"/>
+      <c r="AA141" s="98"/>
+      <c r="AB141" s="98"/>
+      <c r="AC141" s="98"/>
+      <c r="AD141" s="98"/>
+      <c r="AE141" s="98"/>
+      <c r="AF141" s="98"/>
+      <c r="AG141" s="98"/>
+      <c r="AH141" s="98"/>
+      <c r="AI141" s="98"/>
+      <c r="AJ141" s="98"/>
+      <c r="AK141" s="98"/>
+      <c r="AL141" s="98"/>
+      <c r="AM141" s="98"/>
+      <c r="AN141" s="98"/>
+      <c r="AO141" s="98"/>
+      <c r="AP141" s="98"/>
+      <c r="AQ141" s="98"/>
+      <c r="AR141" s="98"/>
+      <c r="AS141" s="98"/>
+      <c r="AT141" s="98"/>
+      <c r="AU141" s="98"/>
+      <c r="AV141" s="98"/>
+      <c r="AW141" s="98"/>
+      <c r="AX141" s="98"/>
+      <c r="AY141" s="98"/>
+      <c r="AZ141" s="98"/>
+      <c r="BA141" s="98"/>
     </row>
     <row r="142" spans="1:53">
       <c r="A142" s="51" t="s">
@@ -13725,62 +13731,62 @@
       <c r="B166" s="17">
         <v>8</v>
       </c>
-      <c r="C166" s="106" t="s">
+      <c r="C166" s="94" t="s">
         <v>30</v>
       </c>
-      <c r="D166" s="107"/>
-      <c r="E166" s="107"/>
-      <c r="F166" s="107"/>
-      <c r="G166" s="107"/>
-      <c r="H166" s="107"/>
-      <c r="I166" s="107"/>
-      <c r="J166" s="107"/>
-      <c r="K166" s="107"/>
-      <c r="L166" s="107"/>
-      <c r="M166" s="107"/>
-      <c r="N166" s="107"/>
-      <c r="O166" s="107"/>
-      <c r="P166" s="108"/>
-      <c r="Q166" s="109" t="str">
+      <c r="D166" s="95"/>
+      <c r="E166" s="95"/>
+      <c r="F166" s="95"/>
+      <c r="G166" s="95"/>
+      <c r="H166" s="95"/>
+      <c r="I166" s="95"/>
+      <c r="J166" s="95"/>
+      <c r="K166" s="95"/>
+      <c r="L166" s="95"/>
+      <c r="M166" s="95"/>
+      <c r="N166" s="95"/>
+      <c r="O166" s="95"/>
+      <c r="P166" s="96"/>
+      <c r="Q166" s="97" t="str">
         <f>VLOOKUP(B166,'SPECIFY(Đặc Tả)(1)'!$A$5:$BA$33,2,0)</f>
         <v>Lập DS các đội ở các hạng đấu</v>
       </c>
-      <c r="R166" s="110"/>
-      <c r="S166" s="110"/>
-      <c r="T166" s="110"/>
-      <c r="U166" s="110"/>
-      <c r="V166" s="110"/>
-      <c r="W166" s="110"/>
-      <c r="X166" s="110"/>
-      <c r="Y166" s="110"/>
-      <c r="Z166" s="110"/>
-      <c r="AA166" s="110"/>
-      <c r="AB166" s="110"/>
-      <c r="AC166" s="110"/>
-      <c r="AD166" s="110"/>
-      <c r="AE166" s="110"/>
-      <c r="AF166" s="110"/>
-      <c r="AG166" s="110"/>
-      <c r="AH166" s="110"/>
-      <c r="AI166" s="110"/>
-      <c r="AJ166" s="110"/>
-      <c r="AK166" s="110"/>
-      <c r="AL166" s="110"/>
-      <c r="AM166" s="110"/>
-      <c r="AN166" s="110"/>
-      <c r="AO166" s="110"/>
-      <c r="AP166" s="110"/>
-      <c r="AQ166" s="110"/>
-      <c r="AR166" s="110"/>
-      <c r="AS166" s="110"/>
-      <c r="AT166" s="110"/>
-      <c r="AU166" s="110"/>
-      <c r="AV166" s="110"/>
-      <c r="AW166" s="110"/>
-      <c r="AX166" s="110"/>
-      <c r="AY166" s="110"/>
-      <c r="AZ166" s="110"/>
-      <c r="BA166" s="110"/>
+      <c r="R166" s="98"/>
+      <c r="S166" s="98"/>
+      <c r="T166" s="98"/>
+      <c r="U166" s="98"/>
+      <c r="V166" s="98"/>
+      <c r="W166" s="98"/>
+      <c r="X166" s="98"/>
+      <c r="Y166" s="98"/>
+      <c r="Z166" s="98"/>
+      <c r="AA166" s="98"/>
+      <c r="AB166" s="98"/>
+      <c r="AC166" s="98"/>
+      <c r="AD166" s="98"/>
+      <c r="AE166" s="98"/>
+      <c r="AF166" s="98"/>
+      <c r="AG166" s="98"/>
+      <c r="AH166" s="98"/>
+      <c r="AI166" s="98"/>
+      <c r="AJ166" s="98"/>
+      <c r="AK166" s="98"/>
+      <c r="AL166" s="98"/>
+      <c r="AM166" s="98"/>
+      <c r="AN166" s="98"/>
+      <c r="AO166" s="98"/>
+      <c r="AP166" s="98"/>
+      <c r="AQ166" s="98"/>
+      <c r="AR166" s="98"/>
+      <c r="AS166" s="98"/>
+      <c r="AT166" s="98"/>
+      <c r="AU166" s="98"/>
+      <c r="AV166" s="98"/>
+      <c r="AW166" s="98"/>
+      <c r="AX166" s="98"/>
+      <c r="AY166" s="98"/>
+      <c r="AZ166" s="98"/>
+      <c r="BA166" s="98"/>
     </row>
     <row r="167" spans="1:53">
       <c r="A167" s="51" t="s">
@@ -15118,62 +15124,62 @@
       <c r="B191" s="17">
         <v>9</v>
       </c>
-      <c r="C191" s="106" t="s">
+      <c r="C191" s="94" t="s">
         <v>30</v>
       </c>
-      <c r="D191" s="107"/>
-      <c r="E191" s="107"/>
-      <c r="F191" s="107"/>
-      <c r="G191" s="107"/>
-      <c r="H191" s="107"/>
-      <c r="I191" s="107"/>
-      <c r="J191" s="107"/>
-      <c r="K191" s="107"/>
-      <c r="L191" s="107"/>
-      <c r="M191" s="107"/>
-      <c r="N191" s="107"/>
-      <c r="O191" s="107"/>
-      <c r="P191" s="108"/>
-      <c r="Q191" s="109" t="str">
+      <c r="D191" s="95"/>
+      <c r="E191" s="95"/>
+      <c r="F191" s="95"/>
+      <c r="G191" s="95"/>
+      <c r="H191" s="95"/>
+      <c r="I191" s="95"/>
+      <c r="J191" s="95"/>
+      <c r="K191" s="95"/>
+      <c r="L191" s="95"/>
+      <c r="M191" s="95"/>
+      <c r="N191" s="95"/>
+      <c r="O191" s="95"/>
+      <c r="P191" s="96"/>
+      <c r="Q191" s="97" t="str">
         <f>VLOOKUP(B191,'SPECIFY(Đặc Tả)(1)'!$A$5:$BA$33,2,0)</f>
         <v>Lập DS các đội dự cup quốc gia</v>
       </c>
-      <c r="R191" s="110"/>
-      <c r="S191" s="110"/>
-      <c r="T191" s="110"/>
-      <c r="U191" s="110"/>
-      <c r="V191" s="110"/>
-      <c r="W191" s="110"/>
-      <c r="X191" s="110"/>
-      <c r="Y191" s="110"/>
-      <c r="Z191" s="110"/>
-      <c r="AA191" s="110"/>
-      <c r="AB191" s="110"/>
-      <c r="AC191" s="110"/>
-      <c r="AD191" s="110"/>
-      <c r="AE191" s="110"/>
-      <c r="AF191" s="110"/>
-      <c r="AG191" s="110"/>
-      <c r="AH191" s="110"/>
-      <c r="AI191" s="110"/>
-      <c r="AJ191" s="110"/>
-      <c r="AK191" s="110"/>
-      <c r="AL191" s="110"/>
-      <c r="AM191" s="110"/>
-      <c r="AN191" s="110"/>
-      <c r="AO191" s="110"/>
-      <c r="AP191" s="110"/>
-      <c r="AQ191" s="110"/>
-      <c r="AR191" s="110"/>
-      <c r="AS191" s="110"/>
-      <c r="AT191" s="110"/>
-      <c r="AU191" s="110"/>
-      <c r="AV191" s="110"/>
-      <c r="AW191" s="110"/>
-      <c r="AX191" s="110"/>
-      <c r="AY191" s="110"/>
-      <c r="AZ191" s="110"/>
-      <c r="BA191" s="110"/>
+      <c r="R191" s="98"/>
+      <c r="S191" s="98"/>
+      <c r="T191" s="98"/>
+      <c r="U191" s="98"/>
+      <c r="V191" s="98"/>
+      <c r="W191" s="98"/>
+      <c r="X191" s="98"/>
+      <c r="Y191" s="98"/>
+      <c r="Z191" s="98"/>
+      <c r="AA191" s="98"/>
+      <c r="AB191" s="98"/>
+      <c r="AC191" s="98"/>
+      <c r="AD191" s="98"/>
+      <c r="AE191" s="98"/>
+      <c r="AF191" s="98"/>
+      <c r="AG191" s="98"/>
+      <c r="AH191" s="98"/>
+      <c r="AI191" s="98"/>
+      <c r="AJ191" s="98"/>
+      <c r="AK191" s="98"/>
+      <c r="AL191" s="98"/>
+      <c r="AM191" s="98"/>
+      <c r="AN191" s="98"/>
+      <c r="AO191" s="98"/>
+      <c r="AP191" s="98"/>
+      <c r="AQ191" s="98"/>
+      <c r="AR191" s="98"/>
+      <c r="AS191" s="98"/>
+      <c r="AT191" s="98"/>
+      <c r="AU191" s="98"/>
+      <c r="AV191" s="98"/>
+      <c r="AW191" s="98"/>
+      <c r="AX191" s="98"/>
+      <c r="AY191" s="98"/>
+      <c r="AZ191" s="98"/>
+      <c r="BA191" s="98"/>
     </row>
     <row r="192" spans="1:53">
       <c r="A192" s="51" t="s">
@@ -16511,62 +16517,62 @@
       <c r="B216" s="17">
         <v>10</v>
       </c>
-      <c r="C216" s="106" t="s">
+      <c r="C216" s="94" t="s">
         <v>30</v>
       </c>
-      <c r="D216" s="107"/>
-      <c r="E216" s="107"/>
-      <c r="F216" s="107"/>
-      <c r="G216" s="107"/>
-      <c r="H216" s="107"/>
-      <c r="I216" s="107"/>
-      <c r="J216" s="107"/>
-      <c r="K216" s="107"/>
-      <c r="L216" s="107"/>
-      <c r="M216" s="107"/>
-      <c r="N216" s="107"/>
-      <c r="O216" s="107"/>
-      <c r="P216" s="108"/>
-      <c r="Q216" s="109" t="str">
+      <c r="D216" s="95"/>
+      <c r="E216" s="95"/>
+      <c r="F216" s="95"/>
+      <c r="G216" s="95"/>
+      <c r="H216" s="95"/>
+      <c r="I216" s="95"/>
+      <c r="J216" s="95"/>
+      <c r="K216" s="95"/>
+      <c r="L216" s="95"/>
+      <c r="M216" s="95"/>
+      <c r="N216" s="95"/>
+      <c r="O216" s="95"/>
+      <c r="P216" s="96"/>
+      <c r="Q216" s="97" t="str">
         <f>VLOOKUP(B216,'SPECIFY(Đặc Tả)(1)'!$A$5:$BA$33,2,0)</f>
         <v>Lập DS các đội dự cup châu lục</v>
       </c>
-      <c r="R216" s="110"/>
-      <c r="S216" s="110"/>
-      <c r="T216" s="110"/>
-      <c r="U216" s="110"/>
-      <c r="V216" s="110"/>
-      <c r="W216" s="110"/>
-      <c r="X216" s="110"/>
-      <c r="Y216" s="110"/>
-      <c r="Z216" s="110"/>
-      <c r="AA216" s="110"/>
-      <c r="AB216" s="110"/>
-      <c r="AC216" s="110"/>
-      <c r="AD216" s="110"/>
-      <c r="AE216" s="110"/>
-      <c r="AF216" s="110"/>
-      <c r="AG216" s="110"/>
-      <c r="AH216" s="110"/>
-      <c r="AI216" s="110"/>
-      <c r="AJ216" s="110"/>
-      <c r="AK216" s="110"/>
-      <c r="AL216" s="110"/>
-      <c r="AM216" s="110"/>
-      <c r="AN216" s="110"/>
-      <c r="AO216" s="110"/>
-      <c r="AP216" s="110"/>
-      <c r="AQ216" s="110"/>
-      <c r="AR216" s="110"/>
-      <c r="AS216" s="110"/>
-      <c r="AT216" s="110"/>
-      <c r="AU216" s="110"/>
-      <c r="AV216" s="110"/>
-      <c r="AW216" s="110"/>
-      <c r="AX216" s="110"/>
-      <c r="AY216" s="110"/>
-      <c r="AZ216" s="110"/>
-      <c r="BA216" s="110"/>
+      <c r="R216" s="98"/>
+      <c r="S216" s="98"/>
+      <c r="T216" s="98"/>
+      <c r="U216" s="98"/>
+      <c r="V216" s="98"/>
+      <c r="W216" s="98"/>
+      <c r="X216" s="98"/>
+      <c r="Y216" s="98"/>
+      <c r="Z216" s="98"/>
+      <c r="AA216" s="98"/>
+      <c r="AB216" s="98"/>
+      <c r="AC216" s="98"/>
+      <c r="AD216" s="98"/>
+      <c r="AE216" s="98"/>
+      <c r="AF216" s="98"/>
+      <c r="AG216" s="98"/>
+      <c r="AH216" s="98"/>
+      <c r="AI216" s="98"/>
+      <c r="AJ216" s="98"/>
+      <c r="AK216" s="98"/>
+      <c r="AL216" s="98"/>
+      <c r="AM216" s="98"/>
+      <c r="AN216" s="98"/>
+      <c r="AO216" s="98"/>
+      <c r="AP216" s="98"/>
+      <c r="AQ216" s="98"/>
+      <c r="AR216" s="98"/>
+      <c r="AS216" s="98"/>
+      <c r="AT216" s="98"/>
+      <c r="AU216" s="98"/>
+      <c r="AV216" s="98"/>
+      <c r="AW216" s="98"/>
+      <c r="AX216" s="98"/>
+      <c r="AY216" s="98"/>
+      <c r="AZ216" s="98"/>
+      <c r="BA216" s="98"/>
     </row>
     <row r="217" spans="1:53">
       <c r="A217" s="51" t="s">
@@ -17904,62 +17910,62 @@
       <c r="B241" s="17">
         <v>11</v>
       </c>
-      <c r="C241" s="106" t="s">
+      <c r="C241" s="94" t="s">
         <v>30</v>
       </c>
-      <c r="D241" s="107"/>
-      <c r="E241" s="107"/>
-      <c r="F241" s="107"/>
-      <c r="G241" s="107"/>
-      <c r="H241" s="107"/>
-      <c r="I241" s="107"/>
-      <c r="J241" s="107"/>
-      <c r="K241" s="107"/>
-      <c r="L241" s="107"/>
-      <c r="M241" s="107"/>
-      <c r="N241" s="107"/>
-      <c r="O241" s="107"/>
-      <c r="P241" s="108"/>
-      <c r="Q241" s="109" t="str">
+      <c r="D241" s="95"/>
+      <c r="E241" s="95"/>
+      <c r="F241" s="95"/>
+      <c r="G241" s="95"/>
+      <c r="H241" s="95"/>
+      <c r="I241" s="95"/>
+      <c r="J241" s="95"/>
+      <c r="K241" s="95"/>
+      <c r="L241" s="95"/>
+      <c r="M241" s="95"/>
+      <c r="N241" s="95"/>
+      <c r="O241" s="95"/>
+      <c r="P241" s="96"/>
+      <c r="Q241" s="97" t="str">
         <f>VLOOKUP(B241,'SPECIFY(Đặc Tả)(1)'!$A$5:$BA$33,2,0)</f>
         <v>Thay đổi quy định</v>
       </c>
-      <c r="R241" s="110"/>
-      <c r="S241" s="110"/>
-      <c r="T241" s="110"/>
-      <c r="U241" s="110"/>
-      <c r="V241" s="110"/>
-      <c r="W241" s="110"/>
-      <c r="X241" s="110"/>
-      <c r="Y241" s="110"/>
-      <c r="Z241" s="110"/>
-      <c r="AA241" s="110"/>
-      <c r="AB241" s="110"/>
-      <c r="AC241" s="110"/>
-      <c r="AD241" s="110"/>
-      <c r="AE241" s="110"/>
-      <c r="AF241" s="110"/>
-      <c r="AG241" s="110"/>
-      <c r="AH241" s="110"/>
-      <c r="AI241" s="110"/>
-      <c r="AJ241" s="110"/>
-      <c r="AK241" s="110"/>
-      <c r="AL241" s="110"/>
-      <c r="AM241" s="110"/>
-      <c r="AN241" s="110"/>
-      <c r="AO241" s="110"/>
-      <c r="AP241" s="110"/>
-      <c r="AQ241" s="110"/>
-      <c r="AR241" s="110"/>
-      <c r="AS241" s="110"/>
-      <c r="AT241" s="110"/>
-      <c r="AU241" s="110"/>
-      <c r="AV241" s="110"/>
-      <c r="AW241" s="110"/>
-      <c r="AX241" s="110"/>
-      <c r="AY241" s="110"/>
-      <c r="AZ241" s="110"/>
-      <c r="BA241" s="110"/>
+      <c r="R241" s="98"/>
+      <c r="S241" s="98"/>
+      <c r="T241" s="98"/>
+      <c r="U241" s="98"/>
+      <c r="V241" s="98"/>
+      <c r="W241" s="98"/>
+      <c r="X241" s="98"/>
+      <c r="Y241" s="98"/>
+      <c r="Z241" s="98"/>
+      <c r="AA241" s="98"/>
+      <c r="AB241" s="98"/>
+      <c r="AC241" s="98"/>
+      <c r="AD241" s="98"/>
+      <c r="AE241" s="98"/>
+      <c r="AF241" s="98"/>
+      <c r="AG241" s="98"/>
+      <c r="AH241" s="98"/>
+      <c r="AI241" s="98"/>
+      <c r="AJ241" s="98"/>
+      <c r="AK241" s="98"/>
+      <c r="AL241" s="98"/>
+      <c r="AM241" s="98"/>
+      <c r="AN241" s="98"/>
+      <c r="AO241" s="98"/>
+      <c r="AP241" s="98"/>
+      <c r="AQ241" s="98"/>
+      <c r="AR241" s="98"/>
+      <c r="AS241" s="98"/>
+      <c r="AT241" s="98"/>
+      <c r="AU241" s="98"/>
+      <c r="AV241" s="98"/>
+      <c r="AW241" s="98"/>
+      <c r="AX241" s="98"/>
+      <c r="AY241" s="98"/>
+      <c r="AZ241" s="98"/>
+      <c r="BA241" s="98"/>
     </row>
     <row r="242" spans="1:53">
       <c r="A242" s="51" t="s">
@@ -19347,6 +19353,23 @@
     </row>
   </sheetData>
   <mergeCells count="29">
+    <mergeCell ref="A1:O1"/>
+    <mergeCell ref="P1:AH1"/>
+    <mergeCell ref="AI1:AM1"/>
+    <mergeCell ref="AN1:BA1"/>
+    <mergeCell ref="AI2:AM2"/>
+    <mergeCell ref="AN2:BA2"/>
+    <mergeCell ref="C91:P91"/>
+    <mergeCell ref="Q91:BA91"/>
+    <mergeCell ref="A3:H3"/>
+    <mergeCell ref="C4:P4"/>
+    <mergeCell ref="Q4:BA4"/>
+    <mergeCell ref="C26:P26"/>
+    <mergeCell ref="Q26:BA26"/>
+    <mergeCell ref="C40:P40"/>
+    <mergeCell ref="Q40:BA40"/>
+    <mergeCell ref="C65:P65"/>
+    <mergeCell ref="Q65:BA65"/>
     <mergeCell ref="C216:P216"/>
     <mergeCell ref="Q216:BA216"/>
     <mergeCell ref="C241:P241"/>
@@ -19359,30 +19382,13 @@
     <mergeCell ref="Q166:BA166"/>
     <mergeCell ref="C191:P191"/>
     <mergeCell ref="Q191:BA191"/>
-    <mergeCell ref="C91:P91"/>
-    <mergeCell ref="Q91:BA91"/>
-    <mergeCell ref="A3:H3"/>
-    <mergeCell ref="C4:P4"/>
-    <mergeCell ref="Q4:BA4"/>
-    <mergeCell ref="C26:P26"/>
-    <mergeCell ref="Q26:BA26"/>
-    <mergeCell ref="C40:P40"/>
-    <mergeCell ref="Q40:BA40"/>
-    <mergeCell ref="C65:P65"/>
-    <mergeCell ref="Q65:BA65"/>
-    <mergeCell ref="A1:O1"/>
-    <mergeCell ref="P1:AH1"/>
-    <mergeCell ref="AI1:AM1"/>
-    <mergeCell ref="AN1:BA1"/>
-    <mergeCell ref="AI2:AM2"/>
-    <mergeCell ref="AN2:BA2"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="0" orientation="portrait" horizontalDpi="0" verticalDpi="0" copies="0"/>
+  <pageSetup orientation="portrait" horizontalDpi="200" verticalDpi="200" copies="0" r:id="rId1"/>
   <headerFooter>
     <oddHeader>&amp;CSPECIFY USE CASE</oddHeader>
   </headerFooter>
-  <legacyDrawing r:id="rId1"/>
+  <legacyDrawing r:id="rId2"/>
 </worksheet>
 </file>
 

</xml_diff>